<commit_message>
Fix dublicating vehicles, make service not write telematics data with null coordinates
</commit_message>
<xml_diff>
--- a/directories/Сапсай_Коми_2025.xlsx
+++ b/directories/Сапсай_Коми_2025.xlsx
@@ -1,25 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
-  <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
-  </bookViews>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <workbookPr/>
   <sheets>
-    <sheet name="Лист1" sheetId="1" r:id="rId1"/>
+    <sheet state="visible" name="Лист1" sheetId="1" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <definedNames/>
+  <calcPr/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
+    <ext uri="GoogleSheetsCustomDataVersion2">
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="huc0C84iKlsury5cjBWKSvaslpOXMVohxjlqbVfEjVk="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="343">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="344">
   <si>
     <t>ГАУ РК "КОМИ ЛЕСОПОЖАРНЫЙ ЦЕНТР"</t>
   </si>
@@ -39,6 +36,12 @@
     <t>Остановлен</t>
   </si>
   <si>
+    <t>Госномер</t>
+  </si>
+  <si>
+    <t>IMEI</t>
+  </si>
+  <si>
     <t>О810СМ11</t>
   </si>
   <si>
@@ -51,6 +54,9 @@
     <t>863071014474792</t>
   </si>
   <si>
+    <t>9223372036854775807</t>
+  </si>
+  <si>
     <t>О787НК11</t>
   </si>
   <si>
@@ -288,126 +294,126 @@
     <t>Р483ОЕ11</t>
   </si>
   <si>
+    <t>Р488ОЕ11</t>
+  </si>
+  <si>
+    <t>354515100884963</t>
+  </si>
+  <si>
+    <t>Р504ОЕ11</t>
+  </si>
+  <si>
+    <t>354515100885242</t>
+  </si>
+  <si>
+    <t>Р075НУ11</t>
+  </si>
+  <si>
+    <t>352555102931489</t>
+  </si>
+  <si>
+    <t>2049МА11</t>
+  </si>
+  <si>
+    <t>352555102929228</t>
+  </si>
+  <si>
+    <t>2048МА11</t>
+  </si>
+  <si>
+    <t>352555102934301</t>
+  </si>
+  <si>
+    <t>Р513РХ11</t>
+  </si>
+  <si>
+    <t>862531045214385</t>
+  </si>
+  <si>
+    <t>Р655СА11</t>
+  </si>
+  <si>
+    <t>862531045214245</t>
+  </si>
+  <si>
+    <t>Р316СК11</t>
+  </si>
+  <si>
+    <t>862531049019632</t>
+  </si>
+  <si>
+    <t>Р586СК11</t>
+  </si>
+  <si>
+    <t>862531042159138</t>
+  </si>
+  <si>
+    <t>Р543СК11</t>
+  </si>
+  <si>
+    <t>862531042213455</t>
+  </si>
+  <si>
+    <t>Р137ТМ11</t>
+  </si>
+  <si>
+    <t>862531049127641</t>
+  </si>
+  <si>
+    <t>Р493ТМ11</t>
+  </si>
+  <si>
+    <t>866795033883743</t>
+  </si>
+  <si>
+    <t>Р453ТМ11</t>
+  </si>
+  <si>
+    <t>862531048082383</t>
+  </si>
+  <si>
+    <t>Р110ТО11</t>
+  </si>
+  <si>
+    <t>353465072463829</t>
+  </si>
+  <si>
+    <t>Р956ТН11</t>
+  </si>
+  <si>
+    <t>353465072484569</t>
+  </si>
+  <si>
+    <t>Р848ТН11</t>
+  </si>
+  <si>
+    <t>863071014460015</t>
+  </si>
+  <si>
+    <t>Р141НУ11</t>
+  </si>
+  <si>
+    <t>868184062237386</t>
+  </si>
+  <si>
+    <t>1091МА11</t>
+  </si>
+  <si>
+    <t>863071014348368</t>
+  </si>
+  <si>
+    <t>Р516УЕ11</t>
+  </si>
+  <si>
+    <t>866854055252228</t>
+  </si>
+  <si>
+    <t>О066НК11</t>
+  </si>
+  <si>
     <t>352555102933345</t>
   </si>
   <si>
-    <t>Р488ОЕ11</t>
-  </si>
-  <si>
-    <t>354515100884963</t>
-  </si>
-  <si>
-    <t>Р504ОЕ11</t>
-  </si>
-  <si>
-    <t>354515100885242</t>
-  </si>
-  <si>
-    <t>Р075НУ11</t>
-  </si>
-  <si>
-    <t>352555102931489</t>
-  </si>
-  <si>
-    <t>2049МА11</t>
-  </si>
-  <si>
-    <t>352555102929228</t>
-  </si>
-  <si>
-    <t>2048МА11</t>
-  </si>
-  <si>
-    <t>352555102934301</t>
-  </si>
-  <si>
-    <t>Р513РХ11</t>
-  </si>
-  <si>
-    <t>862531045214385</t>
-  </si>
-  <si>
-    <t>Р655СА11</t>
-  </si>
-  <si>
-    <t>862531045214245</t>
-  </si>
-  <si>
-    <t>Р316СК11</t>
-  </si>
-  <si>
-    <t>862531049019632</t>
-  </si>
-  <si>
-    <t>Р586СК11</t>
-  </si>
-  <si>
-    <t>862531042159138</t>
-  </si>
-  <si>
-    <t>Р543СК11</t>
-  </si>
-  <si>
-    <t>862531042213455</t>
-  </si>
-  <si>
-    <t>Р137ТМ11</t>
-  </si>
-  <si>
-    <t>862531049127641</t>
-  </si>
-  <si>
-    <t>Р493ТМ11</t>
-  </si>
-  <si>
-    <t>866795033883743</t>
-  </si>
-  <si>
-    <t>Р453ТМ11</t>
-  </si>
-  <si>
-    <t>862531048082383</t>
-  </si>
-  <si>
-    <t>Р110ТО11</t>
-  </si>
-  <si>
-    <t>353465072463829</t>
-  </si>
-  <si>
-    <t>Р956ТН11</t>
-  </si>
-  <si>
-    <t>353465072484569</t>
-  </si>
-  <si>
-    <t>Р848ТН11</t>
-  </si>
-  <si>
-    <t>863071014460015</t>
-  </si>
-  <si>
-    <t>Р141НУ11</t>
-  </si>
-  <si>
-    <t>868184062237386</t>
-  </si>
-  <si>
-    <t>1091МА11</t>
-  </si>
-  <si>
-    <t>863071014348368</t>
-  </si>
-  <si>
-    <t>Р516УЕ11</t>
-  </si>
-  <si>
-    <t>866854055252228</t>
-  </si>
-  <si>
-    <t>О066НК11</t>
-  </si>
-  <si>
     <t>Р730УХ11</t>
   </si>
   <si>
@@ -1042,24 +1048,27 @@
   </si>
   <si>
     <t>866567061241817</t>
-  </si>
-  <si>
-    <t>Госномер</t>
-  </si>
-  <si>
-    <t>IMEI</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <fonts count="3">
     <font>
-      <sz val="11"/>
+      <sz val="11.0"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11.0"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -1068,56 +1077,51 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="gray125"/>
+      <patternFill patternType="lightGray"/>
     </fill>
   </fills>
   <borders count="1">
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
+  <cellXfs count="4">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle xfId="0" name="Normal" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
   <a:themeElements>
-    <a:clrScheme name="Стандартная">
+    <a:clrScheme name="Sheets">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:srgbClr val="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:srgbClr val="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="44546A"/>
+        <a:srgbClr val="000000"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
+        <a:srgbClr val="FFFFFF"/>
       </a:lt2>
       <a:accent1>
         <a:srgbClr val="5B9BD5"/>
@@ -1141,82 +1145,22 @@
         <a:srgbClr val="0563C1"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="954F72"/>
+        <a:srgbClr val="0563C1"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Стандартная">
+    <a:fontScheme name="Sheets">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック Light"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线 Light"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface="Calibri"/>
+        <a:cs typeface="Calibri"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface="Calibri"/>
+        <a:cs typeface="Calibri"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Стандартная">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1354,30 +1298,32 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I169"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <pageSetUpPr/>
+  </sheetPr>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
-    <col min="7" max="7" width="20.7109375" customWidth="1"/>
+    <col customWidth="1" min="1" max="1" width="36.86"/>
+    <col customWidth="1" min="2" max="2" width="113.29"/>
+    <col customWidth="1" min="3" max="3" width="6.43"/>
+    <col customWidth="1" min="4" max="4" width="18.14"/>
+    <col customWidth="1" min="5" max="5" width="7.29"/>
+    <col customWidth="1" min="6" max="6" width="11.71"/>
+    <col customWidth="1" min="7" max="7" width="11.14"/>
+    <col customWidth="1" min="8" max="8" width="17.0"/>
+    <col customWidth="1" min="9" max="9" width="21.29"/>
+    <col customWidth="1" min="10" max="26" width="8.71"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1397,14 +1343,14 @@
         <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>341</v>
+        <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>342</v>
+        <v>7</v>
       </c>
       <c r="I1" s="1"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -1412,14 +1358,21 @@
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I2" s="1"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+      <c r="I2" s="2">
+        <f>LEN("863071014463084")</f>
+        <v>15</v>
+      </c>
+      <c r="J2" s="3">
+        <f>LEN("9223372036854775807")</f>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -1427,14 +1380,16 @@
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="I3" s="1"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -1442,14 +1397,14 @@
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="I4" s="1"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -1457,14 +1412,14 @@
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="I5" s="1"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -1472,14 +1427,14 @@
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
       <c r="G6" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="I6" s="1"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -1487,14 +1442,14 @@
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="I7" s="1"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -1502,14 +1457,14 @@
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
       <c r="G8" s="1" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="I8" s="1"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -1517,14 +1472,14 @@
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="I9" s="1"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -1532,14 +1487,14 @@
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
       <c r="G10" s="1" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="I10" s="1"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -1547,14 +1502,14 @@
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
       <c r="G11" s="1" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="I11" s="1"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -1562,14 +1517,14 @@
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
       <c r="G12" s="1" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="I12" s="1"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -1577,14 +1532,14 @@
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
       <c r="G13" s="1" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="I13" s="1"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -1592,14 +1547,14 @@
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
       <c r="G14" s="1" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="I14" s="1"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -1607,14 +1562,14 @@
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
       <c r="G15" s="1" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="I15" s="1"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -1622,14 +1577,14 @@
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
       <c r="G16" s="1" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="I16" s="1"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -1637,14 +1592,14 @@
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
       <c r="G17" s="1" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="I17" s="1"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -1652,14 +1607,14 @@
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
       <c r="G18" s="1" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="I18" s="1"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -1667,14 +1622,14 @@
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
       <c r="G19" s="1" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="I19" s="1"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -1682,14 +1637,14 @@
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
       <c r="G20" s="1" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="I20" s="1"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" ht="15.75" customHeight="1">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -1697,14 +1652,14 @@
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
       <c r="G21" s="1" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="I21" s="1"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" ht="15.75" customHeight="1">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -1712,14 +1667,14 @@
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
       <c r="G22" s="1" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="I22" s="1"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" ht="15.75" customHeight="1">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -1727,14 +1682,14 @@
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
       <c r="G23" s="1" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="I23" s="1"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" ht="15.75" customHeight="1">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -1742,14 +1697,14 @@
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
       <c r="G24" s="1" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="I24" s="1"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" ht="15.75" customHeight="1">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -1757,14 +1712,14 @@
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
       <c r="G25" s="1" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="I25" s="1"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" ht="15.75" customHeight="1">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -1772,14 +1727,14 @@
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
       <c r="G26" s="1" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="I26" s="1"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" ht="15.75" customHeight="1">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
@@ -1787,14 +1742,14 @@
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
       <c r="G27" s="1" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="I27" s="1"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" ht="15.75" customHeight="1">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
@@ -1802,14 +1757,14 @@
       <c r="E28" s="1"/>
       <c r="F28" s="1"/>
       <c r="G28" s="1" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="I28" s="1"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" ht="15.75" customHeight="1">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
@@ -1817,14 +1772,14 @@
       <c r="E29" s="1"/>
       <c r="F29" s="1"/>
       <c r="G29" s="1" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="I29" s="1"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" ht="15.75" customHeight="1">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
@@ -1832,14 +1787,14 @@
       <c r="E30" s="1"/>
       <c r="F30" s="1"/>
       <c r="G30" s="1" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="I30" s="1"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" ht="15.75" customHeight="1">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
@@ -1847,14 +1802,14 @@
       <c r="E31" s="1"/>
       <c r="F31" s="1"/>
       <c r="G31" s="1" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="I31" s="1"/>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" ht="15.75" customHeight="1">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
@@ -1862,14 +1817,14 @@
       <c r="E32" s="1"/>
       <c r="F32" s="1"/>
       <c r="G32" s="1" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="I32" s="1"/>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" ht="15.75" customHeight="1">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
@@ -1877,14 +1832,14 @@
       <c r="E33" s="1"/>
       <c r="F33" s="1"/>
       <c r="G33" s="1" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="I33" s="1"/>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" ht="15.75" customHeight="1">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
@@ -1892,14 +1847,14 @@
       <c r="E34" s="1"/>
       <c r="F34" s="1"/>
       <c r="G34" s="1" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="I34" s="1"/>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" ht="15.75" customHeight="1">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
@@ -1907,14 +1862,14 @@
       <c r="E35" s="1"/>
       <c r="F35" s="1"/>
       <c r="G35" s="1" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="I35" s="1"/>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" ht="15.75" customHeight="1">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
@@ -1922,14 +1877,14 @@
       <c r="E36" s="1"/>
       <c r="F36" s="1"/>
       <c r="G36" s="1" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="I36" s="1"/>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" ht="15.75" customHeight="1">
       <c r="A37" s="1"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
@@ -1937,14 +1892,14 @@
       <c r="E37" s="1"/>
       <c r="F37" s="1"/>
       <c r="G37" s="1" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="I37" s="1"/>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="38" ht="15.75" customHeight="1">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
@@ -1952,14 +1907,14 @@
       <c r="E38" s="1"/>
       <c r="F38" s="1"/>
       <c r="G38" s="1" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="I38" s="1"/>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="39" ht="15.75" customHeight="1">
       <c r="A39" s="1"/>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
@@ -1967,14 +1922,14 @@
       <c r="E39" s="1"/>
       <c r="F39" s="1"/>
       <c r="G39" s="1" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="I39" s="1"/>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="40" ht="15.75" customHeight="1">
       <c r="A40" s="1"/>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
@@ -1982,14 +1937,14 @@
       <c r="E40" s="1"/>
       <c r="F40" s="1"/>
       <c r="G40" s="1" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="H40" s="1" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="I40" s="1"/>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="41" ht="15.75" customHeight="1">
       <c r="A41" s="1"/>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
@@ -1997,14 +1952,14 @@
       <c r="E41" s="1"/>
       <c r="F41" s="1"/>
       <c r="G41" s="1" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="H41" s="1" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="I41" s="1"/>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="42" ht="15.75" customHeight="1">
       <c r="A42" s="1"/>
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
@@ -2012,14 +1967,14 @@
       <c r="E42" s="1"/>
       <c r="F42" s="1"/>
       <c r="G42" s="1" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="H42" s="1" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="I42" s="1"/>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="43" ht="15.75" customHeight="1">
       <c r="A43" s="1"/>
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
@@ -2027,14 +1982,14 @@
       <c r="E43" s="1"/>
       <c r="F43" s="1"/>
       <c r="G43" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="H43" s="1" t="s">
-        <v>89</v>
+        <v>91</v>
+      </c>
+      <c r="H43" s="2">
+        <v>8.68184067539471E14</v>
       </c>
       <c r="I43" s="1"/>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="44" ht="15.75" customHeight="1">
       <c r="A44" s="1"/>
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
@@ -2042,14 +1997,14 @@
       <c r="E44" s="1"/>
       <c r="F44" s="1"/>
       <c r="G44" s="1" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="H44" s="1" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="I44" s="1"/>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="45" ht="15.75" customHeight="1">
       <c r="A45" s="1"/>
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
@@ -2057,14 +2012,14 @@
       <c r="E45" s="1"/>
       <c r="F45" s="1"/>
       <c r="G45" s="1" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="H45" s="1" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="I45" s="1"/>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="46" ht="15.75" customHeight="1">
       <c r="A46" s="1"/>
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
@@ -2072,14 +2027,14 @@
       <c r="E46" s="1"/>
       <c r="F46" s="1"/>
       <c r="G46" s="1" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="H46" s="1" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="I46" s="1"/>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="47" ht="15.75" customHeight="1">
       <c r="A47" s="1"/>
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
@@ -2087,14 +2042,14 @@
       <c r="E47" s="1"/>
       <c r="F47" s="1"/>
       <c r="G47" s="1" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="H47" s="1" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="I47" s="1"/>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="48" ht="15.75" customHeight="1">
       <c r="A48" s="1"/>
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
@@ -2102,14 +2057,14 @@
       <c r="E48" s="1"/>
       <c r="F48" s="1"/>
       <c r="G48" s="1" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="H48" s="1" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="I48" s="1"/>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="49" ht="15.75" customHeight="1">
       <c r="A49" s="1"/>
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
@@ -2117,14 +2072,14 @@
       <c r="E49" s="1"/>
       <c r="F49" s="1"/>
       <c r="G49" s="1" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="H49" s="1" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="I49" s="1"/>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="50" ht="15.75" customHeight="1">
       <c r="A50" s="1"/>
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
@@ -2132,14 +2087,14 @@
       <c r="E50" s="1"/>
       <c r="F50" s="1"/>
       <c r="G50" s="1" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="H50" s="1" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="I50" s="1"/>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="51" ht="15.75" customHeight="1">
       <c r="A51" s="1"/>
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
@@ -2147,14 +2102,14 @@
       <c r="E51" s="1"/>
       <c r="F51" s="1"/>
       <c r="G51" s="1" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="H51" s="1" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="I51" s="1"/>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="52" ht="15.75" customHeight="1">
       <c r="A52" s="1"/>
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
@@ -2162,14 +2117,14 @@
       <c r="E52" s="1"/>
       <c r="F52" s="1"/>
       <c r="G52" s="1" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="H52" s="1" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="I52" s="1"/>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="53" ht="15.75" customHeight="1">
       <c r="A53" s="1"/>
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
@@ -2177,14 +2132,14 @@
       <c r="E53" s="1"/>
       <c r="F53" s="1"/>
       <c r="G53" s="1" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="H53" s="1" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="I53" s="1"/>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="54" ht="15.75" customHeight="1">
       <c r="A54" s="1"/>
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>
@@ -2192,14 +2147,14 @@
       <c r="E54" s="1"/>
       <c r="F54" s="1"/>
       <c r="G54" s="1" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="H54" s="1" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="I54" s="1"/>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="55" ht="15.75" customHeight="1">
       <c r="A55" s="1"/>
       <c r="B55" s="1"/>
       <c r="C55" s="1"/>
@@ -2207,14 +2162,14 @@
       <c r="E55" s="1"/>
       <c r="F55" s="1"/>
       <c r="G55" s="1" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="H55" s="1" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="I55" s="1"/>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="56" ht="15.75" customHeight="1">
       <c r="A56" s="1"/>
       <c r="B56" s="1"/>
       <c r="C56" s="1"/>
@@ -2222,14 +2177,14 @@
       <c r="E56" s="1"/>
       <c r="F56" s="1"/>
       <c r="G56" s="1" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="H56" s="1" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="I56" s="1"/>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="57" ht="15.75" customHeight="1">
       <c r="A57" s="1"/>
       <c r="B57" s="1"/>
       <c r="C57" s="1"/>
@@ -2237,14 +2192,14 @@
       <c r="E57" s="1"/>
       <c r="F57" s="1"/>
       <c r="G57" s="1" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="H57" s="1" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="I57" s="1"/>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="58" ht="15.75" customHeight="1">
       <c r="A58" s="1"/>
       <c r="B58" s="1"/>
       <c r="C58" s="1"/>
@@ -2252,14 +2207,14 @@
       <c r="E58" s="1"/>
       <c r="F58" s="1"/>
       <c r="G58" s="1" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="H58" s="1" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="I58" s="1"/>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="59" ht="15.75" customHeight="1">
       <c r="A59" s="1"/>
       <c r="B59" s="1"/>
       <c r="C59" s="1"/>
@@ -2267,14 +2222,14 @@
       <c r="E59" s="1"/>
       <c r="F59" s="1"/>
       <c r="G59" s="1" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="H59" s="1" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="I59" s="1"/>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="60" ht="15.75" customHeight="1">
       <c r="A60" s="1"/>
       <c r="B60" s="1"/>
       <c r="C60" s="1"/>
@@ -2282,14 +2237,14 @@
       <c r="E60" s="1"/>
       <c r="F60" s="1"/>
       <c r="G60" s="1" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="H60" s="1" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="I60" s="1"/>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="61" ht="15.75" customHeight="1">
       <c r="A61" s="1"/>
       <c r="B61" s="1"/>
       <c r="C61" s="1"/>
@@ -2297,14 +2252,14 @@
       <c r="E61" s="1"/>
       <c r="F61" s="1"/>
       <c r="G61" s="1" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="H61" s="1" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="I61" s="1"/>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="62" ht="15.75" customHeight="1">
       <c r="A62" s="1"/>
       <c r="B62" s="1"/>
       <c r="C62" s="1"/>
@@ -2312,14 +2267,14 @@
       <c r="E62" s="1"/>
       <c r="F62" s="1"/>
       <c r="G62" s="1" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="H62" s="1" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="I62" s="1"/>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="63" ht="15.75" customHeight="1">
       <c r="A63" s="1"/>
       <c r="B63" s="1"/>
       <c r="C63" s="1"/>
@@ -2327,14 +2282,14 @@
       <c r="E63" s="1"/>
       <c r="F63" s="1"/>
       <c r="G63" s="1" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="H63" s="1" t="s">
-        <v>89</v>
+        <v>131</v>
       </c>
       <c r="I63" s="1"/>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="64" ht="15.75" customHeight="1">
       <c r="A64" s="1"/>
       <c r="B64" s="1"/>
       <c r="C64" s="1"/>
@@ -2342,14 +2297,14 @@
       <c r="E64" s="1"/>
       <c r="F64" s="1"/>
       <c r="G64" s="1" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="H64" s="1" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="I64" s="1"/>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="65" ht="15.75" customHeight="1">
       <c r="A65" s="1"/>
       <c r="B65" s="1"/>
       <c r="C65" s="1"/>
@@ -2357,14 +2312,14 @@
       <c r="E65" s="1"/>
       <c r="F65" s="1"/>
       <c r="G65" s="1" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="H65" s="1" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="I65" s="1"/>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="66" ht="15.75" customHeight="1">
       <c r="A66" s="1"/>
       <c r="B66" s="1"/>
       <c r="C66" s="1"/>
@@ -2372,14 +2327,14 @@
       <c r="E66" s="1"/>
       <c r="F66" s="1"/>
       <c r="G66" s="1" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="H66" s="1" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="I66" s="1"/>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="67" ht="15.75" customHeight="1">
       <c r="A67" s="1"/>
       <c r="B67" s="1"/>
       <c r="C67" s="1"/>
@@ -2387,14 +2342,14 @@
       <c r="E67" s="1"/>
       <c r="F67" s="1"/>
       <c r="G67" s="1" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="H67" s="1" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="I67" s="1"/>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="68" ht="15.75" customHeight="1">
       <c r="A68" s="1"/>
       <c r="B68" s="1"/>
       <c r="C68" s="1"/>
@@ -2402,14 +2357,14 @@
       <c r="E68" s="1"/>
       <c r="F68" s="1"/>
       <c r="G68" s="1" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="H68" s="1" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="I68" s="1"/>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="69" ht="15.75" customHeight="1">
       <c r="A69" s="1"/>
       <c r="B69" s="1"/>
       <c r="C69" s="1"/>
@@ -2417,14 +2372,14 @@
       <c r="E69" s="1"/>
       <c r="F69" s="1"/>
       <c r="G69" s="1" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="H69" s="1" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="I69" s="1"/>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="70" ht="15.75" customHeight="1">
       <c r="A70" s="1"/>
       <c r="B70" s="1"/>
       <c r="C70" s="1"/>
@@ -2432,14 +2387,14 @@
       <c r="E70" s="1"/>
       <c r="F70" s="1"/>
       <c r="G70" s="1" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="H70" s="1" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="I70" s="1"/>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="71" ht="15.75" customHeight="1">
       <c r="A71" s="1"/>
       <c r="B71" s="1"/>
       <c r="C71" s="1"/>
@@ -2447,14 +2402,14 @@
       <c r="E71" s="1"/>
       <c r="F71" s="1"/>
       <c r="G71" s="1" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="H71" s="1" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="I71" s="1"/>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="72" ht="15.75" customHeight="1">
       <c r="A72" s="1"/>
       <c r="B72" s="1"/>
       <c r="C72" s="1"/>
@@ -2462,14 +2417,14 @@
       <c r="E72" s="1"/>
       <c r="F72" s="1"/>
       <c r="G72" s="1" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="H72" s="1" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="I72" s="1"/>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="73" ht="15.75" customHeight="1">
       <c r="A73" s="1"/>
       <c r="B73" s="1"/>
       <c r="C73" s="1"/>
@@ -2477,14 +2432,14 @@
       <c r="E73" s="1"/>
       <c r="F73" s="1"/>
       <c r="G73" s="1" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="H73" s="1" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="I73" s="1"/>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="74" ht="15.75" customHeight="1">
       <c r="A74" s="1"/>
       <c r="B74" s="1"/>
       <c r="C74" s="1"/>
@@ -2492,14 +2447,14 @@
       <c r="E74" s="1"/>
       <c r="F74" s="1"/>
       <c r="G74" s="1" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="H74" s="1" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="I74" s="1"/>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="75" ht="15.75" customHeight="1">
       <c r="A75" s="1"/>
       <c r="B75" s="1"/>
       <c r="C75" s="1"/>
@@ -2507,14 +2462,14 @@
       <c r="E75" s="1"/>
       <c r="F75" s="1"/>
       <c r="G75" s="1" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="H75" s="1" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="I75" s="1"/>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="76" ht="15.75" customHeight="1">
       <c r="A76" s="1"/>
       <c r="B76" s="1"/>
       <c r="C76" s="1"/>
@@ -2522,14 +2477,14 @@
       <c r="E76" s="1"/>
       <c r="F76" s="1"/>
       <c r="G76" s="1" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="H76" s="1" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="I76" s="1"/>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="77" ht="15.75" customHeight="1">
       <c r="A77" s="1"/>
       <c r="B77" s="1"/>
       <c r="C77" s="1"/>
@@ -2537,14 +2492,14 @@
       <c r="E77" s="1"/>
       <c r="F77" s="1"/>
       <c r="G77" s="1" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="H77" s="1" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="I77" s="1"/>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="78" ht="15.75" customHeight="1">
       <c r="A78" s="1"/>
       <c r="B78" s="1"/>
       <c r="C78" s="1"/>
@@ -2552,14 +2507,14 @@
       <c r="E78" s="1"/>
       <c r="F78" s="1"/>
       <c r="G78" s="1" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="H78" s="1" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="I78" s="1"/>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="79" ht="15.75" customHeight="1">
       <c r="A79" s="1"/>
       <c r="B79" s="1"/>
       <c r="C79" s="1"/>
@@ -2567,14 +2522,14 @@
       <c r="E79" s="1"/>
       <c r="F79" s="1"/>
       <c r="G79" s="1" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="H79" s="1" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="I79" s="1"/>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="80" ht="15.75" customHeight="1">
       <c r="A80" s="1"/>
       <c r="B80" s="1"/>
       <c r="C80" s="1"/>
@@ -2582,14 +2537,14 @@
       <c r="E80" s="1"/>
       <c r="F80" s="1"/>
       <c r="G80" s="1" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="H80" s="1" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="I80" s="1"/>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="81" ht="15.75" customHeight="1">
       <c r="A81" s="1"/>
       <c r="B81" s="1"/>
       <c r="C81" s="1"/>
@@ -2597,14 +2552,14 @@
       <c r="E81" s="1"/>
       <c r="F81" s="1"/>
       <c r="G81" s="1" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="H81" s="1" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="I81" s="1"/>
     </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="82" ht="15.75" customHeight="1">
       <c r="A82" s="1"/>
       <c r="B82" s="1"/>
       <c r="C82" s="1"/>
@@ -2612,14 +2567,14 @@
       <c r="E82" s="1"/>
       <c r="F82" s="1"/>
       <c r="G82" s="1" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="H82" s="1" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="I82" s="1"/>
     </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="83" ht="15.75" customHeight="1">
       <c r="A83" s="1"/>
       <c r="B83" s="1"/>
       <c r="C83" s="1"/>
@@ -2627,14 +2582,14 @@
       <c r="E83" s="1"/>
       <c r="F83" s="1"/>
       <c r="G83" s="1" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="H83" s="1" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="I83" s="1"/>
     </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="84" ht="15.75" customHeight="1">
       <c r="A84" s="1"/>
       <c r="B84" s="1"/>
       <c r="C84" s="1"/>
@@ -2642,14 +2597,14 @@
       <c r="E84" s="1"/>
       <c r="F84" s="1"/>
       <c r="G84" s="1" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="H84" s="1" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="I84" s="1"/>
     </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="85" ht="15.75" customHeight="1">
       <c r="A85" s="1"/>
       <c r="B85" s="1"/>
       <c r="C85" s="1"/>
@@ -2657,14 +2612,14 @@
       <c r="E85" s="1"/>
       <c r="F85" s="1"/>
       <c r="G85" s="1" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="H85" s="1" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="I85" s="1"/>
     </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="86" ht="15.75" customHeight="1">
       <c r="A86" s="1"/>
       <c r="B86" s="1"/>
       <c r="C86" s="1"/>
@@ -2672,14 +2627,14 @@
       <c r="E86" s="1"/>
       <c r="F86" s="1"/>
       <c r="G86" s="1" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="H86" s="1" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="I86" s="1"/>
     </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="87" ht="15.75" customHeight="1">
       <c r="A87" s="1"/>
       <c r="B87" s="1"/>
       <c r="C87" s="1"/>
@@ -2687,14 +2642,14 @@
       <c r="E87" s="1"/>
       <c r="F87" s="1"/>
       <c r="G87" s="1" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="H87" s="1" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="I87" s="1"/>
     </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="88" ht="15.75" customHeight="1">
       <c r="A88" s="1"/>
       <c r="B88" s="1"/>
       <c r="C88" s="1"/>
@@ -2702,14 +2657,14 @@
       <c r="E88" s="1"/>
       <c r="F88" s="1"/>
       <c r="G88" s="1" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="H88" s="1" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="I88" s="1"/>
     </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="89" ht="15.75" customHeight="1">
       <c r="A89" s="1"/>
       <c r="B89" s="1"/>
       <c r="C89" s="1"/>
@@ -2717,14 +2672,14 @@
       <c r="E89" s="1"/>
       <c r="F89" s="1"/>
       <c r="G89" s="1" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="H89" s="1" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="I89" s="1"/>
     </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="90" ht="15.75" customHeight="1">
       <c r="A90" s="1"/>
       <c r="B90" s="1"/>
       <c r="C90" s="1"/>
@@ -2732,14 +2687,14 @@
       <c r="E90" s="1"/>
       <c r="F90" s="1"/>
       <c r="G90" s="1" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="H90" s="1" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="I90" s="1"/>
     </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="91" ht="15.75" customHeight="1">
       <c r="A91" s="1"/>
       <c r="B91" s="1"/>
       <c r="C91" s="1"/>
@@ -2747,14 +2702,14 @@
       <c r="E91" s="1"/>
       <c r="F91" s="1"/>
       <c r="G91" s="1" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="H91" s="1" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="I91" s="1"/>
     </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="92" ht="15.75" customHeight="1">
       <c r="A92" s="1"/>
       <c r="B92" s="1"/>
       <c r="C92" s="1"/>
@@ -2762,14 +2717,14 @@
       <c r="E92" s="1"/>
       <c r="F92" s="1"/>
       <c r="G92" s="1" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="H92" s="1" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="I92" s="1"/>
     </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="93" ht="15.75" customHeight="1">
       <c r="A93" s="1"/>
       <c r="B93" s="1"/>
       <c r="C93" s="1"/>
@@ -2777,14 +2732,14 @@
       <c r="E93" s="1"/>
       <c r="F93" s="1"/>
       <c r="G93" s="1" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="H93" s="1" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="I93" s="1"/>
     </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="94" ht="15.75" customHeight="1">
       <c r="A94" s="1"/>
       <c r="B94" s="1"/>
       <c r="C94" s="1"/>
@@ -2792,14 +2747,14 @@
       <c r="E94" s="1"/>
       <c r="F94" s="1"/>
       <c r="G94" s="1" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="H94" s="1" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="I94" s="1"/>
     </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="95" ht="15.75" customHeight="1">
       <c r="A95" s="1"/>
       <c r="B95" s="1"/>
       <c r="C95" s="1"/>
@@ -2807,14 +2762,14 @@
       <c r="E95" s="1"/>
       <c r="F95" s="1"/>
       <c r="G95" s="1" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="H95" s="1" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="I95" s="1"/>
     </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="96" ht="15.75" customHeight="1">
       <c r="A96" s="1"/>
       <c r="B96" s="1"/>
       <c r="C96" s="1"/>
@@ -2822,14 +2777,14 @@
       <c r="E96" s="1"/>
       <c r="F96" s="1"/>
       <c r="G96" s="1" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="H96" s="1" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="I96" s="1"/>
     </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="97" ht="15.75" customHeight="1">
       <c r="A97" s="1"/>
       <c r="B97" s="1"/>
       <c r="C97" s="1"/>
@@ -2837,14 +2792,14 @@
       <c r="E97" s="1"/>
       <c r="F97" s="1"/>
       <c r="G97" s="1" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="H97" s="1" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="I97" s="1"/>
     </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="98" ht="15.75" customHeight="1">
       <c r="A98" s="1"/>
       <c r="B98" s="1"/>
       <c r="C98" s="1"/>
@@ -2852,14 +2807,14 @@
       <c r="E98" s="1"/>
       <c r="F98" s="1"/>
       <c r="G98" s="1" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="H98" s="1" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="I98" s="1"/>
     </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="99" ht="15.75" customHeight="1">
       <c r="A99" s="1"/>
       <c r="B99" s="1"/>
       <c r="C99" s="1"/>
@@ -2867,14 +2822,14 @@
       <c r="E99" s="1"/>
       <c r="F99" s="1"/>
       <c r="G99" s="1" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="H99" s="1" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="I99" s="1"/>
     </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="100" ht="15.75" customHeight="1">
       <c r="A100" s="1"/>
       <c r="B100" s="1"/>
       <c r="C100" s="1"/>
@@ -2882,14 +2837,14 @@
       <c r="E100" s="1"/>
       <c r="F100" s="1"/>
       <c r="G100" s="1" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="H100" s="1" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="I100" s="1"/>
     </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="101" ht="15.75" customHeight="1">
       <c r="A101" s="1"/>
       <c r="B101" s="1"/>
       <c r="C101" s="1"/>
@@ -2897,14 +2852,14 @@
       <c r="E101" s="1"/>
       <c r="F101" s="1"/>
       <c r="G101" s="1" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="H101" s="1" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="I101" s="1"/>
     </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="102" ht="15.75" customHeight="1">
       <c r="A102" s="1"/>
       <c r="B102" s="1"/>
       <c r="C102" s="1"/>
@@ -2912,14 +2867,14 @@
       <c r="E102" s="1"/>
       <c r="F102" s="1"/>
       <c r="G102" s="1" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="H102" s="1" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="I102" s="1"/>
     </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="103" ht="15.75" customHeight="1">
       <c r="A103" s="1"/>
       <c r="B103" s="1"/>
       <c r="C103" s="1"/>
@@ -2927,14 +2882,14 @@
       <c r="E103" s="1"/>
       <c r="F103" s="1"/>
       <c r="G103" s="1" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="H103" s="1" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="I103" s="1"/>
     </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="104" ht="15.75" customHeight="1">
       <c r="A104" s="1"/>
       <c r="B104" s="1"/>
       <c r="C104" s="1"/>
@@ -2942,14 +2897,14 @@
       <c r="E104" s="1"/>
       <c r="F104" s="1"/>
       <c r="G104" s="1" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="H104" s="1" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="I104" s="1"/>
     </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="105" ht="15.75" customHeight="1">
       <c r="A105" s="1"/>
       <c r="B105" s="1"/>
       <c r="C105" s="1"/>
@@ -2957,14 +2912,14 @@
       <c r="E105" s="1"/>
       <c r="F105" s="1"/>
       <c r="G105" s="1" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="H105" s="1" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="I105" s="1"/>
     </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="106" ht="15.75" customHeight="1">
       <c r="A106" s="1"/>
       <c r="B106" s="1"/>
       <c r="C106" s="1"/>
@@ -2972,14 +2927,14 @@
       <c r="E106" s="1"/>
       <c r="F106" s="1"/>
       <c r="G106" s="1" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="H106" s="1" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
       <c r="I106" s="1"/>
     </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="107" ht="15.75" customHeight="1">
       <c r="A107" s="1"/>
       <c r="B107" s="1"/>
       <c r="C107" s="1"/>
@@ -2987,14 +2942,14 @@
       <c r="E107" s="1"/>
       <c r="F107" s="1"/>
       <c r="G107" s="1" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="H107" s="1" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="I107" s="1"/>
     </row>
-    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="108" ht="15.75" customHeight="1">
       <c r="A108" s="1"/>
       <c r="B108" s="1"/>
       <c r="C108" s="1"/>
@@ -3002,14 +2957,14 @@
       <c r="E108" s="1"/>
       <c r="F108" s="1"/>
       <c r="G108" s="1" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="H108" s="1" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="I108" s="1"/>
     </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="109" ht="15.75" customHeight="1">
       <c r="A109" s="1"/>
       <c r="B109" s="1"/>
       <c r="C109" s="1"/>
@@ -3017,14 +2972,14 @@
       <c r="E109" s="1"/>
       <c r="F109" s="1"/>
       <c r="G109" s="1" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="H109" s="1" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="I109" s="1"/>
     </row>
-    <row r="110" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="110" ht="15.75" customHeight="1">
       <c r="A110" s="1"/>
       <c r="B110" s="1"/>
       <c r="C110" s="1"/>
@@ -3032,14 +2987,14 @@
       <c r="E110" s="1"/>
       <c r="F110" s="1"/>
       <c r="G110" s="1" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
       <c r="H110" s="1" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="I110" s="1"/>
     </row>
-    <row r="111" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="111" ht="15.75" customHeight="1">
       <c r="A111" s="1"/>
       <c r="B111" s="1"/>
       <c r="C111" s="1"/>
@@ -3047,14 +3002,14 @@
       <c r="E111" s="1"/>
       <c r="F111" s="1"/>
       <c r="G111" s="1" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
       <c r="H111" s="1" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
       <c r="I111" s="1"/>
     </row>
-    <row r="112" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="112" ht="15.75" customHeight="1">
       <c r="A112" s="1"/>
       <c r="B112" s="1"/>
       <c r="C112" s="1"/>
@@ -3062,14 +3017,14 @@
       <c r="E112" s="1"/>
       <c r="F112" s="1"/>
       <c r="G112" s="1" t="s">
-        <v>225</v>
+        <v>228</v>
       </c>
       <c r="H112" s="1" t="s">
-        <v>226</v>
+        <v>229</v>
       </c>
       <c r="I112" s="1"/>
     </row>
-    <row r="113" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="113" ht="15.75" customHeight="1">
       <c r="A113" s="1"/>
       <c r="B113" s="1"/>
       <c r="C113" s="1"/>
@@ -3077,14 +3032,14 @@
       <c r="E113" s="1"/>
       <c r="F113" s="1"/>
       <c r="G113" s="1" t="s">
-        <v>227</v>
+        <v>230</v>
       </c>
       <c r="H113" s="1" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
       <c r="I113" s="1"/>
     </row>
-    <row r="114" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="114" ht="15.75" customHeight="1">
       <c r="A114" s="1"/>
       <c r="B114" s="1"/>
       <c r="C114" s="1"/>
@@ -3092,14 +3047,14 @@
       <c r="E114" s="1"/>
       <c r="F114" s="1"/>
       <c r="G114" s="1" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
       <c r="H114" s="1" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
       <c r="I114" s="1"/>
     </row>
-    <row r="115" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="115" ht="15.75" customHeight="1">
       <c r="A115" s="1"/>
       <c r="B115" s="1"/>
       <c r="C115" s="1"/>
@@ -3107,14 +3062,14 @@
       <c r="E115" s="1"/>
       <c r="F115" s="1"/>
       <c r="G115" s="1" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="H115" s="1" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="I115" s="1"/>
     </row>
-    <row r="116" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="116" ht="15.75" customHeight="1">
       <c r="A116" s="1"/>
       <c r="B116" s="1"/>
       <c r="C116" s="1"/>
@@ -3122,14 +3077,14 @@
       <c r="E116" s="1"/>
       <c r="F116" s="1"/>
       <c r="G116" s="1" t="s">
-        <v>233</v>
+        <v>236</v>
       </c>
       <c r="H116" s="1" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
       <c r="I116" s="1"/>
     </row>
-    <row r="117" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="117" ht="15.75" customHeight="1">
       <c r="A117" s="1"/>
       <c r="B117" s="1"/>
       <c r="C117" s="1"/>
@@ -3137,14 +3092,14 @@
       <c r="E117" s="1"/>
       <c r="F117" s="1"/>
       <c r="G117" s="1" t="s">
-        <v>235</v>
+        <v>238</v>
       </c>
       <c r="H117" s="1" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
       <c r="I117" s="1"/>
     </row>
-    <row r="118" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="118" ht="15.75" customHeight="1">
       <c r="A118" s="1"/>
       <c r="B118" s="1"/>
       <c r="C118" s="1"/>
@@ -3152,14 +3107,14 @@
       <c r="E118" s="1"/>
       <c r="F118" s="1"/>
       <c r="G118" s="1" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
       <c r="H118" s="1" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
       <c r="I118" s="1"/>
     </row>
-    <row r="119" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="119" ht="15.75" customHeight="1">
       <c r="A119" s="1"/>
       <c r="B119" s="1"/>
       <c r="C119" s="1"/>
@@ -3167,14 +3122,14 @@
       <c r="E119" s="1"/>
       <c r="F119" s="1"/>
       <c r="G119" s="1" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="H119" s="1" t="s">
-        <v>240</v>
+        <v>243</v>
       </c>
       <c r="I119" s="1"/>
     </row>
-    <row r="120" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="120" ht="15.75" customHeight="1">
       <c r="A120" s="1"/>
       <c r="B120" s="1"/>
       <c r="C120" s="1"/>
@@ -3182,14 +3137,14 @@
       <c r="E120" s="1"/>
       <c r="F120" s="1"/>
       <c r="G120" s="1" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
       <c r="H120" s="1" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
       <c r="I120" s="1"/>
     </row>
-    <row r="121" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="121" ht="15.75" customHeight="1">
       <c r="A121" s="1"/>
       <c r="B121" s="1"/>
       <c r="C121" s="1"/>
@@ -3197,14 +3152,14 @@
       <c r="E121" s="1"/>
       <c r="F121" s="1"/>
       <c r="G121" s="1" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
       <c r="H121" s="1" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
       <c r="I121" s="1"/>
     </row>
-    <row r="122" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="122" ht="15.75" customHeight="1">
       <c r="A122" s="1"/>
       <c r="B122" s="1"/>
       <c r="C122" s="1"/>
@@ -3212,14 +3167,14 @@
       <c r="E122" s="1"/>
       <c r="F122" s="1"/>
       <c r="G122" s="1" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="H122" s="1" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
       <c r="I122" s="1"/>
     </row>
-    <row r="123" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="123" ht="15.75" customHeight="1">
       <c r="A123" s="1"/>
       <c r="B123" s="1"/>
       <c r="C123" s="1"/>
@@ -3227,14 +3182,14 @@
       <c r="E123" s="1"/>
       <c r="F123" s="1"/>
       <c r="G123" s="1" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
       <c r="H123" s="1" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="I123" s="1"/>
     </row>
-    <row r="124" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="124" ht="15.75" customHeight="1">
       <c r="A124" s="1"/>
       <c r="B124" s="1"/>
       <c r="C124" s="1"/>
@@ -3242,14 +3197,14 @@
       <c r="E124" s="1"/>
       <c r="F124" s="1"/>
       <c r="G124" s="1" t="s">
-        <v>249</v>
+        <v>252</v>
       </c>
       <c r="H124" s="1" t="s">
-        <v>250</v>
+        <v>253</v>
       </c>
       <c r="I124" s="1"/>
     </row>
-    <row r="125" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="125" ht="15.75" customHeight="1">
       <c r="A125" s="1"/>
       <c r="B125" s="1"/>
       <c r="C125" s="1"/>
@@ -3257,14 +3212,14 @@
       <c r="E125" s="1"/>
       <c r="F125" s="1"/>
       <c r="G125" s="1" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="H125" s="1" t="s">
-        <v>252</v>
+        <v>255</v>
       </c>
       <c r="I125" s="1"/>
     </row>
-    <row r="126" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="126" ht="15.75" customHeight="1">
       <c r="A126" s="1"/>
       <c r="B126" s="1"/>
       <c r="C126" s="1"/>
@@ -3272,14 +3227,14 @@
       <c r="E126" s="1"/>
       <c r="F126" s="1"/>
       <c r="G126" s="1" t="s">
-        <v>253</v>
+        <v>256</v>
       </c>
       <c r="H126" s="1" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
       <c r="I126" s="1"/>
     </row>
-    <row r="127" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="127" ht="15.75" customHeight="1">
       <c r="A127" s="1"/>
       <c r="B127" s="1"/>
       <c r="C127" s="1"/>
@@ -3287,14 +3242,14 @@
       <c r="E127" s="1"/>
       <c r="F127" s="1"/>
       <c r="G127" s="1" t="s">
-        <v>255</v>
+        <v>258</v>
       </c>
       <c r="H127" s="1" t="s">
-        <v>256</v>
+        <v>259</v>
       </c>
       <c r="I127" s="1"/>
     </row>
-    <row r="128" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="128" ht="15.75" customHeight="1">
       <c r="A128" s="1"/>
       <c r="B128" s="1"/>
       <c r="C128" s="1"/>
@@ -3302,14 +3257,14 @@
       <c r="E128" s="1"/>
       <c r="F128" s="1"/>
       <c r="G128" s="1" t="s">
-        <v>257</v>
+        <v>260</v>
       </c>
       <c r="H128" s="1" t="s">
-        <v>258</v>
+        <v>261</v>
       </c>
       <c r="I128" s="1"/>
     </row>
-    <row r="129" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="129" ht="15.75" customHeight="1">
       <c r="A129" s="1"/>
       <c r="B129" s="1"/>
       <c r="C129" s="1"/>
@@ -3317,14 +3272,14 @@
       <c r="E129" s="1"/>
       <c r="F129" s="1"/>
       <c r="G129" s="1" t="s">
-        <v>259</v>
+        <v>262</v>
       </c>
       <c r="H129" s="1" t="s">
-        <v>260</v>
+        <v>263</v>
       </c>
       <c r="I129" s="1"/>
     </row>
-    <row r="130" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="130" ht="15.75" customHeight="1">
       <c r="A130" s="1"/>
       <c r="B130" s="1"/>
       <c r="C130" s="1"/>
@@ -3332,14 +3287,14 @@
       <c r="E130" s="1"/>
       <c r="F130" s="1"/>
       <c r="G130" s="1" t="s">
-        <v>261</v>
+        <v>264</v>
       </c>
       <c r="H130" s="1" t="s">
-        <v>262</v>
+        <v>265</v>
       </c>
       <c r="I130" s="1"/>
     </row>
-    <row r="131" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="131" ht="15.75" customHeight="1">
       <c r="A131" s="1"/>
       <c r="B131" s="1"/>
       <c r="C131" s="1"/>
@@ -3347,14 +3302,14 @@
       <c r="E131" s="1"/>
       <c r="F131" s="1"/>
       <c r="G131" s="1" t="s">
-        <v>263</v>
+        <v>266</v>
       </c>
       <c r="H131" s="1" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
       <c r="I131" s="1"/>
     </row>
-    <row r="132" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="132" ht="15.75" customHeight="1">
       <c r="A132" s="1"/>
       <c r="B132" s="1"/>
       <c r="C132" s="1"/>
@@ -3362,14 +3317,14 @@
       <c r="E132" s="1"/>
       <c r="F132" s="1"/>
       <c r="G132" s="1" t="s">
-        <v>265</v>
+        <v>268</v>
       </c>
       <c r="H132" s="1" t="s">
-        <v>266</v>
+        <v>269</v>
       </c>
       <c r="I132" s="1"/>
     </row>
-    <row r="133" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="133" ht="15.75" customHeight="1">
       <c r="A133" s="1"/>
       <c r="B133" s="1"/>
       <c r="C133" s="1"/>
@@ -3377,14 +3332,14 @@
       <c r="E133" s="1"/>
       <c r="F133" s="1"/>
       <c r="G133" s="1" t="s">
-        <v>267</v>
+        <v>270</v>
       </c>
       <c r="H133" s="1" t="s">
-        <v>268</v>
+        <v>271</v>
       </c>
       <c r="I133" s="1"/>
     </row>
-    <row r="134" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="134" ht="15.75" customHeight="1">
       <c r="A134" s="1"/>
       <c r="B134" s="1"/>
       <c r="C134" s="1"/>
@@ -3392,14 +3347,14 @@
       <c r="E134" s="1"/>
       <c r="F134" s="1"/>
       <c r="G134" s="1" t="s">
-        <v>269</v>
+        <v>272</v>
       </c>
       <c r="H134" s="1" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="I134" s="1"/>
     </row>
-    <row r="135" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="135" ht="15.75" customHeight="1">
       <c r="A135" s="1"/>
       <c r="B135" s="1"/>
       <c r="C135" s="1"/>
@@ -3407,14 +3362,14 @@
       <c r="E135" s="1"/>
       <c r="F135" s="1"/>
       <c r="G135" s="1" t="s">
-        <v>271</v>
+        <v>274</v>
       </c>
       <c r="H135" s="1" t="s">
-        <v>272</v>
+        <v>275</v>
       </c>
       <c r="I135" s="1"/>
     </row>
-    <row r="136" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="136" ht="15.75" customHeight="1">
       <c r="A136" s="1"/>
       <c r="B136" s="1"/>
       <c r="C136" s="1"/>
@@ -3422,14 +3377,14 @@
       <c r="E136" s="1"/>
       <c r="F136" s="1"/>
       <c r="G136" s="1" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
       <c r="H136" s="1" t="s">
-        <v>274</v>
+        <v>277</v>
       </c>
       <c r="I136" s="1"/>
     </row>
-    <row r="137" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="137" ht="15.75" customHeight="1">
       <c r="A137" s="1"/>
       <c r="B137" s="1"/>
       <c r="C137" s="1"/>
@@ -3437,14 +3392,14 @@
       <c r="E137" s="1"/>
       <c r="F137" s="1"/>
       <c r="G137" s="1" t="s">
-        <v>275</v>
+        <v>278</v>
       </c>
       <c r="H137" s="1" t="s">
-        <v>276</v>
+        <v>279</v>
       </c>
       <c r="I137" s="1"/>
     </row>
-    <row r="138" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="138" ht="15.75" customHeight="1">
       <c r="A138" s="1"/>
       <c r="B138" s="1"/>
       <c r="C138" s="1"/>
@@ -3452,14 +3407,14 @@
       <c r="E138" s="1"/>
       <c r="F138" s="1"/>
       <c r="G138" s="1" t="s">
-        <v>277</v>
+        <v>280</v>
       </c>
       <c r="H138" s="1" t="s">
-        <v>278</v>
+        <v>281</v>
       </c>
       <c r="I138" s="1"/>
     </row>
-    <row r="139" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="139" ht="15.75" customHeight="1">
       <c r="A139" s="1"/>
       <c r="B139" s="1"/>
       <c r="C139" s="1"/>
@@ -3467,14 +3422,14 @@
       <c r="E139" s="1"/>
       <c r="F139" s="1"/>
       <c r="G139" s="1" t="s">
-        <v>279</v>
+        <v>282</v>
       </c>
       <c r="H139" s="1" t="s">
-        <v>280</v>
+        <v>283</v>
       </c>
       <c r="I139" s="1"/>
     </row>
-    <row r="140" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="140" ht="15.75" customHeight="1">
       <c r="A140" s="1"/>
       <c r="B140" s="1"/>
       <c r="C140" s="1"/>
@@ -3482,14 +3437,14 @@
       <c r="E140" s="1"/>
       <c r="F140" s="1"/>
       <c r="G140" s="1" t="s">
-        <v>281</v>
+        <v>284</v>
       </c>
       <c r="H140" s="1" t="s">
-        <v>282</v>
+        <v>285</v>
       </c>
       <c r="I140" s="1"/>
     </row>
-    <row r="141" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="141" ht="15.75" customHeight="1">
       <c r="A141" s="1"/>
       <c r="B141" s="1"/>
       <c r="C141" s="1"/>
@@ -3497,14 +3452,14 @@
       <c r="E141" s="1"/>
       <c r="F141" s="1"/>
       <c r="G141" s="1" t="s">
-        <v>283</v>
+        <v>286</v>
       </c>
       <c r="H141" s="1" t="s">
-        <v>284</v>
+        <v>287</v>
       </c>
       <c r="I141" s="1"/>
     </row>
-    <row r="142" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="142" ht="15.75" customHeight="1">
       <c r="A142" s="1"/>
       <c r="B142" s="1"/>
       <c r="C142" s="1"/>
@@ -3512,14 +3467,14 @@
       <c r="E142" s="1"/>
       <c r="F142" s="1"/>
       <c r="G142" s="1" t="s">
-        <v>285</v>
+        <v>288</v>
       </c>
       <c r="H142" s="1" t="s">
-        <v>286</v>
+        <v>289</v>
       </c>
       <c r="I142" s="1"/>
     </row>
-    <row r="143" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="143" ht="15.75" customHeight="1">
       <c r="A143" s="1"/>
       <c r="B143" s="1"/>
       <c r="C143" s="1"/>
@@ -3527,14 +3482,14 @@
       <c r="E143" s="1"/>
       <c r="F143" s="1"/>
       <c r="G143" s="1" t="s">
-        <v>287</v>
+        <v>290</v>
       </c>
       <c r="H143" s="1" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="I143" s="1"/>
     </row>
-    <row r="144" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="144" ht="15.75" customHeight="1">
       <c r="A144" s="1"/>
       <c r="B144" s="1"/>
       <c r="C144" s="1"/>
@@ -3542,14 +3497,14 @@
       <c r="E144" s="1"/>
       <c r="F144" s="1"/>
       <c r="G144" s="1" t="s">
-        <v>289</v>
+        <v>292</v>
       </c>
       <c r="H144" s="1" t="s">
-        <v>290</v>
+        <v>293</v>
       </c>
       <c r="I144" s="1"/>
     </row>
-    <row r="145" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="145" ht="15.75" customHeight="1">
       <c r="A145" s="1"/>
       <c r="B145" s="1"/>
       <c r="C145" s="1"/>
@@ -3557,14 +3512,14 @@
       <c r="E145" s="1"/>
       <c r="F145" s="1"/>
       <c r="G145" s="1" t="s">
-        <v>291</v>
+        <v>294</v>
       </c>
       <c r="H145" s="1" t="s">
-        <v>292</v>
+        <v>295</v>
       </c>
       <c r="I145" s="1"/>
     </row>
-    <row r="146" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="146" ht="15.75" customHeight="1">
       <c r="A146" s="1"/>
       <c r="B146" s="1"/>
       <c r="C146" s="1"/>
@@ -3572,14 +3527,14 @@
       <c r="E146" s="1"/>
       <c r="F146" s="1"/>
       <c r="G146" s="1" t="s">
-        <v>293</v>
+        <v>296</v>
       </c>
       <c r="H146" s="1" t="s">
-        <v>294</v>
+        <v>297</v>
       </c>
       <c r="I146" s="1"/>
     </row>
-    <row r="147" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="147" ht="15.75" customHeight="1">
       <c r="A147" s="1"/>
       <c r="B147" s="1"/>
       <c r="C147" s="1"/>
@@ -3587,14 +3542,14 @@
       <c r="E147" s="1"/>
       <c r="F147" s="1"/>
       <c r="G147" s="1" t="s">
-        <v>295</v>
+        <v>298</v>
       </c>
       <c r="H147" s="1" t="s">
-        <v>296</v>
+        <v>299</v>
       </c>
       <c r="I147" s="1"/>
     </row>
-    <row r="148" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="148" ht="15.75" customHeight="1">
       <c r="A148" s="1"/>
       <c r="B148" s="1"/>
       <c r="C148" s="1"/>
@@ -3602,14 +3557,14 @@
       <c r="E148" s="1"/>
       <c r="F148" s="1"/>
       <c r="G148" s="1" t="s">
-        <v>297</v>
+        <v>300</v>
       </c>
       <c r="H148" s="1" t="s">
-        <v>298</v>
+        <v>301</v>
       </c>
       <c r="I148" s="1"/>
     </row>
-    <row r="149" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="149" ht="15.75" customHeight="1">
       <c r="A149" s="1"/>
       <c r="B149" s="1"/>
       <c r="C149" s="1"/>
@@ -3617,14 +3572,14 @@
       <c r="E149" s="1"/>
       <c r="F149" s="1"/>
       <c r="G149" s="1" t="s">
-        <v>299</v>
+        <v>302</v>
       </c>
       <c r="H149" s="1" t="s">
-        <v>300</v>
+        <v>303</v>
       </c>
       <c r="I149" s="1"/>
     </row>
-    <row r="150" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="150" ht="15.75" customHeight="1">
       <c r="A150" s="1"/>
       <c r="B150" s="1"/>
       <c r="C150" s="1"/>
@@ -3632,14 +3587,14 @@
       <c r="E150" s="1"/>
       <c r="F150" s="1"/>
       <c r="G150" s="1" t="s">
-        <v>301</v>
+        <v>304</v>
       </c>
       <c r="H150" s="1" t="s">
-        <v>302</v>
+        <v>305</v>
       </c>
       <c r="I150" s="1"/>
     </row>
-    <row r="151" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="151" ht="15.75" customHeight="1">
       <c r="A151" s="1"/>
       <c r="B151" s="1"/>
       <c r="C151" s="1"/>
@@ -3647,14 +3602,14 @@
       <c r="E151" s="1"/>
       <c r="F151" s="1"/>
       <c r="G151" s="1" t="s">
-        <v>303</v>
+        <v>306</v>
       </c>
       <c r="H151" s="1" t="s">
-        <v>304</v>
+        <v>307</v>
       </c>
       <c r="I151" s="1"/>
     </row>
-    <row r="152" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="152" ht="15.75" customHeight="1">
       <c r="A152" s="1"/>
       <c r="B152" s="1"/>
       <c r="C152" s="1"/>
@@ -3662,14 +3617,14 @@
       <c r="E152" s="1"/>
       <c r="F152" s="1"/>
       <c r="G152" s="1" t="s">
-        <v>305</v>
+        <v>308</v>
       </c>
       <c r="H152" s="1" t="s">
-        <v>306</v>
+        <v>309</v>
       </c>
       <c r="I152" s="1"/>
     </row>
-    <row r="153" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="153" ht="15.75" customHeight="1">
       <c r="A153" s="1"/>
       <c r="B153" s="1"/>
       <c r="C153" s="1"/>
@@ -3677,14 +3632,14 @@
       <c r="E153" s="1"/>
       <c r="F153" s="1"/>
       <c r="G153" s="1" t="s">
-        <v>307</v>
+        <v>310</v>
       </c>
       <c r="H153" s="1" t="s">
-        <v>308</v>
+        <v>311</v>
       </c>
       <c r="I153" s="1"/>
     </row>
-    <row r="154" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="154" ht="15.75" customHeight="1">
       <c r="A154" s="1"/>
       <c r="B154" s="1"/>
       <c r="C154" s="1"/>
@@ -3692,14 +3647,14 @@
       <c r="E154" s="1"/>
       <c r="F154" s="1"/>
       <c r="G154" s="1" t="s">
-        <v>309</v>
+        <v>312</v>
       </c>
       <c r="H154" s="1" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
       <c r="I154" s="1"/>
     </row>
-    <row r="155" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="155" ht="15.75" customHeight="1">
       <c r="A155" s="1"/>
       <c r="B155" s="1"/>
       <c r="C155" s="1"/>
@@ -3707,14 +3662,14 @@
       <c r="E155" s="1"/>
       <c r="F155" s="1"/>
       <c r="G155" s="1" t="s">
-        <v>311</v>
+        <v>314</v>
       </c>
       <c r="H155" s="1" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="I155" s="1"/>
     </row>
-    <row r="156" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="156" ht="15.75" customHeight="1">
       <c r="A156" s="1"/>
       <c r="B156" s="1"/>
       <c r="C156" s="1"/>
@@ -3722,14 +3677,14 @@
       <c r="E156" s="1"/>
       <c r="F156" s="1"/>
       <c r="G156" s="1" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="H156" s="1" t="s">
-        <v>314</v>
+        <v>317</v>
       </c>
       <c r="I156" s="1"/>
     </row>
-    <row r="157" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="157" ht="15.75" customHeight="1">
       <c r="A157" s="1"/>
       <c r="B157" s="1"/>
       <c r="C157" s="1"/>
@@ -3737,14 +3692,14 @@
       <c r="E157" s="1"/>
       <c r="F157" s="1"/>
       <c r="G157" s="1" t="s">
-        <v>315</v>
+        <v>318</v>
       </c>
       <c r="H157" s="1" t="s">
-        <v>316</v>
+        <v>319</v>
       </c>
       <c r="I157" s="1"/>
     </row>
-    <row r="158" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="158" ht="15.75" customHeight="1">
       <c r="A158" s="1"/>
       <c r="B158" s="1"/>
       <c r="C158" s="1"/>
@@ -3752,14 +3707,14 @@
       <c r="E158" s="1"/>
       <c r="F158" s="1"/>
       <c r="G158" s="1" t="s">
-        <v>317</v>
+        <v>320</v>
       </c>
       <c r="H158" s="1" t="s">
-        <v>318</v>
+        <v>321</v>
       </c>
       <c r="I158" s="1"/>
     </row>
-    <row r="159" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="159" ht="15.75" customHeight="1">
       <c r="A159" s="1"/>
       <c r="B159" s="1"/>
       <c r="C159" s="1"/>
@@ -3767,14 +3722,14 @@
       <c r="E159" s="1"/>
       <c r="F159" s="1"/>
       <c r="G159" s="1" t="s">
-        <v>319</v>
+        <v>322</v>
       </c>
       <c r="H159" s="1" t="s">
-        <v>320</v>
+        <v>323</v>
       </c>
       <c r="I159" s="1"/>
     </row>
-    <row r="160" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="160" ht="15.75" customHeight="1">
       <c r="A160" s="1"/>
       <c r="B160" s="1"/>
       <c r="C160" s="1"/>
@@ -3782,14 +3737,14 @@
       <c r="E160" s="1"/>
       <c r="F160" s="1"/>
       <c r="G160" s="1" t="s">
-        <v>321</v>
+        <v>324</v>
       </c>
       <c r="H160" s="1" t="s">
-        <v>322</v>
+        <v>325</v>
       </c>
       <c r="I160" s="1"/>
     </row>
-    <row r="161" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="161" ht="15.75" customHeight="1">
       <c r="A161" s="1"/>
       <c r="B161" s="1"/>
       <c r="C161" s="1"/>
@@ -3797,14 +3752,14 @@
       <c r="E161" s="1"/>
       <c r="F161" s="1"/>
       <c r="G161" s="1" t="s">
-        <v>323</v>
+        <v>326</v>
       </c>
       <c r="H161" s="1" t="s">
-        <v>324</v>
+        <v>327</v>
       </c>
       <c r="I161" s="1"/>
     </row>
-    <row r="162" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="162" ht="15.75" customHeight="1">
       <c r="A162" s="1"/>
       <c r="B162" s="1"/>
       <c r="C162" s="1"/>
@@ -3812,14 +3767,14 @@
       <c r="E162" s="1"/>
       <c r="F162" s="1"/>
       <c r="G162" s="1" t="s">
-        <v>325</v>
+        <v>328</v>
       </c>
       <c r="H162" s="1" t="s">
-        <v>326</v>
+        <v>329</v>
       </c>
       <c r="I162" s="1"/>
     </row>
-    <row r="163" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="163" ht="15.75" customHeight="1">
       <c r="A163" s="1"/>
       <c r="B163" s="1"/>
       <c r="C163" s="1"/>
@@ -3827,14 +3782,14 @@
       <c r="E163" s="1"/>
       <c r="F163" s="1"/>
       <c r="G163" s="1" t="s">
-        <v>327</v>
+        <v>330</v>
       </c>
       <c r="H163" s="1" t="s">
-        <v>328</v>
+        <v>331</v>
       </c>
       <c r="I163" s="1"/>
     </row>
-    <row r="164" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="164" ht="15.75" customHeight="1">
       <c r="A164" s="1"/>
       <c r="B164" s="1"/>
       <c r="C164" s="1"/>
@@ -3842,14 +3797,14 @@
       <c r="E164" s="1"/>
       <c r="F164" s="1"/>
       <c r="G164" s="1" t="s">
-        <v>329</v>
+        <v>332</v>
       </c>
       <c r="H164" s="1" t="s">
-        <v>330</v>
+        <v>333</v>
       </c>
       <c r="I164" s="1"/>
     </row>
-    <row r="165" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="165" ht="15.75" customHeight="1">
       <c r="A165" s="1"/>
       <c r="B165" s="1"/>
       <c r="C165" s="1"/>
@@ -3857,14 +3812,14 @@
       <c r="E165" s="1"/>
       <c r="F165" s="1"/>
       <c r="G165" s="1" t="s">
-        <v>331</v>
+        <v>334</v>
       </c>
       <c r="H165" s="1" t="s">
-        <v>332</v>
+        <v>335</v>
       </c>
       <c r="I165" s="1"/>
     </row>
-    <row r="166" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="166" ht="15.75" customHeight="1">
       <c r="A166" s="1"/>
       <c r="B166" s="1"/>
       <c r="C166" s="1"/>
@@ -3872,14 +3827,14 @@
       <c r="E166" s="1"/>
       <c r="F166" s="1"/>
       <c r="G166" s="1" t="s">
-        <v>333</v>
+        <v>336</v>
       </c>
       <c r="H166" s="1" t="s">
-        <v>334</v>
+        <v>337</v>
       </c>
       <c r="I166" s="1"/>
     </row>
-    <row r="167" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="167" ht="15.75" customHeight="1">
       <c r="A167" s="1"/>
       <c r="B167" s="1"/>
       <c r="C167" s="1"/>
@@ -3887,14 +3842,14 @@
       <c r="E167" s="1"/>
       <c r="F167" s="1"/>
       <c r="G167" s="1" t="s">
-        <v>335</v>
+        <v>338</v>
       </c>
       <c r="H167" s="1" t="s">
-        <v>336</v>
+        <v>339</v>
       </c>
       <c r="I167" s="1"/>
     </row>
-    <row r="168" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="168" ht="15.75" customHeight="1">
       <c r="A168" s="1"/>
       <c r="B168" s="1"/>
       <c r="C168" s="1"/>
@@ -3902,14 +3857,14 @@
       <c r="E168" s="1"/>
       <c r="F168" s="1"/>
       <c r="G168" s="1" t="s">
-        <v>337</v>
+        <v>340</v>
       </c>
       <c r="H168" s="1" t="s">
-        <v>338</v>
+        <v>341</v>
       </c>
       <c r="I168" s="1"/>
     </row>
-    <row r="169" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="169" ht="15.75" customHeight="1">
       <c r="A169" s="1"/>
       <c r="B169" s="1"/>
       <c r="C169" s="1"/>
@@ -3917,14 +3872,848 @@
       <c r="E169" s="1"/>
       <c r="F169" s="1"/>
       <c r="G169" s="1" t="s">
-        <v>339</v>
+        <v>342</v>
       </c>
       <c r="H169" s="1" t="s">
-        <v>340</v>
+        <v>343</v>
       </c>
       <c r="I169" s="1"/>
     </row>
+    <row r="170" ht="15.75" customHeight="1"/>
+    <row r="171" ht="15.75" customHeight="1"/>
+    <row r="172" ht="15.75" customHeight="1"/>
+    <row r="173" ht="15.75" customHeight="1"/>
+    <row r="174" ht="15.75" customHeight="1"/>
+    <row r="175" ht="15.75" customHeight="1"/>
+    <row r="176" ht="15.75" customHeight="1"/>
+    <row r="177" ht="15.75" customHeight="1"/>
+    <row r="178" ht="15.75" customHeight="1"/>
+    <row r="179" ht="15.75" customHeight="1"/>
+    <row r="180" ht="15.75" customHeight="1"/>
+    <row r="181" ht="15.75" customHeight="1"/>
+    <row r="182" ht="15.75" customHeight="1"/>
+    <row r="183" ht="15.75" customHeight="1"/>
+    <row r="184" ht="15.75" customHeight="1"/>
+    <row r="185" ht="15.75" customHeight="1"/>
+    <row r="186" ht="15.75" customHeight="1"/>
+    <row r="187" ht="15.75" customHeight="1"/>
+    <row r="188" ht="15.75" customHeight="1"/>
+    <row r="189" ht="15.75" customHeight="1"/>
+    <row r="190" ht="15.75" customHeight="1"/>
+    <row r="191" ht="15.75" customHeight="1"/>
+    <row r="192" ht="15.75" customHeight="1"/>
+    <row r="193" ht="15.75" customHeight="1"/>
+    <row r="194" ht="15.75" customHeight="1"/>
+    <row r="195" ht="15.75" customHeight="1"/>
+    <row r="196" ht="15.75" customHeight="1"/>
+    <row r="197" ht="15.75" customHeight="1"/>
+    <row r="198" ht="15.75" customHeight="1"/>
+    <row r="199" ht="15.75" customHeight="1"/>
+    <row r="200" ht="15.75" customHeight="1"/>
+    <row r="201" ht="15.75" customHeight="1"/>
+    <row r="202" ht="15.75" customHeight="1"/>
+    <row r="203" ht="15.75" customHeight="1"/>
+    <row r="204" ht="15.75" customHeight="1"/>
+    <row r="205" ht="15.75" customHeight="1"/>
+    <row r="206" ht="15.75" customHeight="1"/>
+    <row r="207" ht="15.75" customHeight="1"/>
+    <row r="208" ht="15.75" customHeight="1"/>
+    <row r="209" ht="15.75" customHeight="1"/>
+    <row r="210" ht="15.75" customHeight="1"/>
+    <row r="211" ht="15.75" customHeight="1"/>
+    <row r="212" ht="15.75" customHeight="1"/>
+    <row r="213" ht="15.75" customHeight="1"/>
+    <row r="214" ht="15.75" customHeight="1"/>
+    <row r="215" ht="15.75" customHeight="1"/>
+    <row r="216" ht="15.75" customHeight="1"/>
+    <row r="217" ht="15.75" customHeight="1"/>
+    <row r="218" ht="15.75" customHeight="1"/>
+    <row r="219" ht="15.75" customHeight="1"/>
+    <row r="220" ht="15.75" customHeight="1"/>
+    <row r="221" ht="15.75" customHeight="1"/>
+    <row r="222" ht="15.75" customHeight="1"/>
+    <row r="223" ht="15.75" customHeight="1"/>
+    <row r="224" ht="15.75" customHeight="1"/>
+    <row r="225" ht="15.75" customHeight="1"/>
+    <row r="226" ht="15.75" customHeight="1"/>
+    <row r="227" ht="15.75" customHeight="1"/>
+    <row r="228" ht="15.75" customHeight="1"/>
+    <row r="229" ht="15.75" customHeight="1"/>
+    <row r="230" ht="15.75" customHeight="1"/>
+    <row r="231" ht="15.75" customHeight="1"/>
+    <row r="232" ht="15.75" customHeight="1"/>
+    <row r="233" ht="15.75" customHeight="1"/>
+    <row r="234" ht="15.75" customHeight="1"/>
+    <row r="235" ht="15.75" customHeight="1"/>
+    <row r="236" ht="15.75" customHeight="1"/>
+    <row r="237" ht="15.75" customHeight="1"/>
+    <row r="238" ht="15.75" customHeight="1"/>
+    <row r="239" ht="15.75" customHeight="1"/>
+    <row r="240" ht="15.75" customHeight="1"/>
+    <row r="241" ht="15.75" customHeight="1"/>
+    <row r="242" ht="15.75" customHeight="1"/>
+    <row r="243" ht="15.75" customHeight="1"/>
+    <row r="244" ht="15.75" customHeight="1"/>
+    <row r="245" ht="15.75" customHeight="1"/>
+    <row r="246" ht="15.75" customHeight="1"/>
+    <row r="247" ht="15.75" customHeight="1"/>
+    <row r="248" ht="15.75" customHeight="1"/>
+    <row r="249" ht="15.75" customHeight="1"/>
+    <row r="250" ht="15.75" customHeight="1"/>
+    <row r="251" ht="15.75" customHeight="1"/>
+    <row r="252" ht="15.75" customHeight="1"/>
+    <row r="253" ht="15.75" customHeight="1"/>
+    <row r="254" ht="15.75" customHeight="1"/>
+    <row r="255" ht="15.75" customHeight="1"/>
+    <row r="256" ht="15.75" customHeight="1"/>
+    <row r="257" ht="15.75" customHeight="1"/>
+    <row r="258" ht="15.75" customHeight="1"/>
+    <row r="259" ht="15.75" customHeight="1"/>
+    <row r="260" ht="15.75" customHeight="1"/>
+    <row r="261" ht="15.75" customHeight="1"/>
+    <row r="262" ht="15.75" customHeight="1"/>
+    <row r="263" ht="15.75" customHeight="1"/>
+    <row r="264" ht="15.75" customHeight="1"/>
+    <row r="265" ht="15.75" customHeight="1"/>
+    <row r="266" ht="15.75" customHeight="1"/>
+    <row r="267" ht="15.75" customHeight="1"/>
+    <row r="268" ht="15.75" customHeight="1"/>
+    <row r="269" ht="15.75" customHeight="1"/>
+    <row r="270" ht="15.75" customHeight="1"/>
+    <row r="271" ht="15.75" customHeight="1"/>
+    <row r="272" ht="15.75" customHeight="1"/>
+    <row r="273" ht="15.75" customHeight="1"/>
+    <row r="274" ht="15.75" customHeight="1"/>
+    <row r="275" ht="15.75" customHeight="1"/>
+    <row r="276" ht="15.75" customHeight="1"/>
+    <row r="277" ht="15.75" customHeight="1"/>
+    <row r="278" ht="15.75" customHeight="1"/>
+    <row r="279" ht="15.75" customHeight="1"/>
+    <row r="280" ht="15.75" customHeight="1"/>
+    <row r="281" ht="15.75" customHeight="1"/>
+    <row r="282" ht="15.75" customHeight="1"/>
+    <row r="283" ht="15.75" customHeight="1"/>
+    <row r="284" ht="15.75" customHeight="1"/>
+    <row r="285" ht="15.75" customHeight="1"/>
+    <row r="286" ht="15.75" customHeight="1"/>
+    <row r="287" ht="15.75" customHeight="1"/>
+    <row r="288" ht="15.75" customHeight="1"/>
+    <row r="289" ht="15.75" customHeight="1"/>
+    <row r="290" ht="15.75" customHeight="1"/>
+    <row r="291" ht="15.75" customHeight="1"/>
+    <row r="292" ht="15.75" customHeight="1"/>
+    <row r="293" ht="15.75" customHeight="1"/>
+    <row r="294" ht="15.75" customHeight="1"/>
+    <row r="295" ht="15.75" customHeight="1"/>
+    <row r="296" ht="15.75" customHeight="1"/>
+    <row r="297" ht="15.75" customHeight="1"/>
+    <row r="298" ht="15.75" customHeight="1"/>
+    <row r="299" ht="15.75" customHeight="1"/>
+    <row r="300" ht="15.75" customHeight="1"/>
+    <row r="301" ht="15.75" customHeight="1"/>
+    <row r="302" ht="15.75" customHeight="1"/>
+    <row r="303" ht="15.75" customHeight="1"/>
+    <row r="304" ht="15.75" customHeight="1"/>
+    <row r="305" ht="15.75" customHeight="1"/>
+    <row r="306" ht="15.75" customHeight="1"/>
+    <row r="307" ht="15.75" customHeight="1"/>
+    <row r="308" ht="15.75" customHeight="1"/>
+    <row r="309" ht="15.75" customHeight="1"/>
+    <row r="310" ht="15.75" customHeight="1"/>
+    <row r="311" ht="15.75" customHeight="1"/>
+    <row r="312" ht="15.75" customHeight="1"/>
+    <row r="313" ht="15.75" customHeight="1"/>
+    <row r="314" ht="15.75" customHeight="1"/>
+    <row r="315" ht="15.75" customHeight="1"/>
+    <row r="316" ht="15.75" customHeight="1"/>
+    <row r="317" ht="15.75" customHeight="1"/>
+    <row r="318" ht="15.75" customHeight="1"/>
+    <row r="319" ht="15.75" customHeight="1"/>
+    <row r="320" ht="15.75" customHeight="1"/>
+    <row r="321" ht="15.75" customHeight="1"/>
+    <row r="322" ht="15.75" customHeight="1"/>
+    <row r="323" ht="15.75" customHeight="1"/>
+    <row r="324" ht="15.75" customHeight="1"/>
+    <row r="325" ht="15.75" customHeight="1"/>
+    <row r="326" ht="15.75" customHeight="1"/>
+    <row r="327" ht="15.75" customHeight="1"/>
+    <row r="328" ht="15.75" customHeight="1"/>
+    <row r="329" ht="15.75" customHeight="1"/>
+    <row r="330" ht="15.75" customHeight="1"/>
+    <row r="331" ht="15.75" customHeight="1"/>
+    <row r="332" ht="15.75" customHeight="1"/>
+    <row r="333" ht="15.75" customHeight="1"/>
+    <row r="334" ht="15.75" customHeight="1"/>
+    <row r="335" ht="15.75" customHeight="1"/>
+    <row r="336" ht="15.75" customHeight="1"/>
+    <row r="337" ht="15.75" customHeight="1"/>
+    <row r="338" ht="15.75" customHeight="1"/>
+    <row r="339" ht="15.75" customHeight="1"/>
+    <row r="340" ht="15.75" customHeight="1"/>
+    <row r="341" ht="15.75" customHeight="1"/>
+    <row r="342" ht="15.75" customHeight="1"/>
+    <row r="343" ht="15.75" customHeight="1"/>
+    <row r="344" ht="15.75" customHeight="1"/>
+    <row r="345" ht="15.75" customHeight="1"/>
+    <row r="346" ht="15.75" customHeight="1"/>
+    <row r="347" ht="15.75" customHeight="1"/>
+    <row r="348" ht="15.75" customHeight="1"/>
+    <row r="349" ht="15.75" customHeight="1"/>
+    <row r="350" ht="15.75" customHeight="1"/>
+    <row r="351" ht="15.75" customHeight="1"/>
+    <row r="352" ht="15.75" customHeight="1"/>
+    <row r="353" ht="15.75" customHeight="1"/>
+    <row r="354" ht="15.75" customHeight="1"/>
+    <row r="355" ht="15.75" customHeight="1"/>
+    <row r="356" ht="15.75" customHeight="1"/>
+    <row r="357" ht="15.75" customHeight="1"/>
+    <row r="358" ht="15.75" customHeight="1"/>
+    <row r="359" ht="15.75" customHeight="1"/>
+    <row r="360" ht="15.75" customHeight="1"/>
+    <row r="361" ht="15.75" customHeight="1"/>
+    <row r="362" ht="15.75" customHeight="1"/>
+    <row r="363" ht="15.75" customHeight="1"/>
+    <row r="364" ht="15.75" customHeight="1"/>
+    <row r="365" ht="15.75" customHeight="1"/>
+    <row r="366" ht="15.75" customHeight="1"/>
+    <row r="367" ht="15.75" customHeight="1"/>
+    <row r="368" ht="15.75" customHeight="1"/>
+    <row r="369" ht="15.75" customHeight="1"/>
+    <row r="370" ht="15.75" customHeight="1"/>
+    <row r="371" ht="15.75" customHeight="1"/>
+    <row r="372" ht="15.75" customHeight="1"/>
+    <row r="373" ht="15.75" customHeight="1"/>
+    <row r="374" ht="15.75" customHeight="1"/>
+    <row r="375" ht="15.75" customHeight="1"/>
+    <row r="376" ht="15.75" customHeight="1"/>
+    <row r="377" ht="15.75" customHeight="1"/>
+    <row r="378" ht="15.75" customHeight="1"/>
+    <row r="379" ht="15.75" customHeight="1"/>
+    <row r="380" ht="15.75" customHeight="1"/>
+    <row r="381" ht="15.75" customHeight="1"/>
+    <row r="382" ht="15.75" customHeight="1"/>
+    <row r="383" ht="15.75" customHeight="1"/>
+    <row r="384" ht="15.75" customHeight="1"/>
+    <row r="385" ht="15.75" customHeight="1"/>
+    <row r="386" ht="15.75" customHeight="1"/>
+    <row r="387" ht="15.75" customHeight="1"/>
+    <row r="388" ht="15.75" customHeight="1"/>
+    <row r="389" ht="15.75" customHeight="1"/>
+    <row r="390" ht="15.75" customHeight="1"/>
+    <row r="391" ht="15.75" customHeight="1"/>
+    <row r="392" ht="15.75" customHeight="1"/>
+    <row r="393" ht="15.75" customHeight="1"/>
+    <row r="394" ht="15.75" customHeight="1"/>
+    <row r="395" ht="15.75" customHeight="1"/>
+    <row r="396" ht="15.75" customHeight="1"/>
+    <row r="397" ht="15.75" customHeight="1"/>
+    <row r="398" ht="15.75" customHeight="1"/>
+    <row r="399" ht="15.75" customHeight="1"/>
+    <row r="400" ht="15.75" customHeight="1"/>
+    <row r="401" ht="15.75" customHeight="1"/>
+    <row r="402" ht="15.75" customHeight="1"/>
+    <row r="403" ht="15.75" customHeight="1"/>
+    <row r="404" ht="15.75" customHeight="1"/>
+    <row r="405" ht="15.75" customHeight="1"/>
+    <row r="406" ht="15.75" customHeight="1"/>
+    <row r="407" ht="15.75" customHeight="1"/>
+    <row r="408" ht="15.75" customHeight="1"/>
+    <row r="409" ht="15.75" customHeight="1"/>
+    <row r="410" ht="15.75" customHeight="1"/>
+    <row r="411" ht="15.75" customHeight="1"/>
+    <row r="412" ht="15.75" customHeight="1"/>
+    <row r="413" ht="15.75" customHeight="1"/>
+    <row r="414" ht="15.75" customHeight="1"/>
+    <row r="415" ht="15.75" customHeight="1"/>
+    <row r="416" ht="15.75" customHeight="1"/>
+    <row r="417" ht="15.75" customHeight="1"/>
+    <row r="418" ht="15.75" customHeight="1"/>
+    <row r="419" ht="15.75" customHeight="1"/>
+    <row r="420" ht="15.75" customHeight="1"/>
+    <row r="421" ht="15.75" customHeight="1"/>
+    <row r="422" ht="15.75" customHeight="1"/>
+    <row r="423" ht="15.75" customHeight="1"/>
+    <row r="424" ht="15.75" customHeight="1"/>
+    <row r="425" ht="15.75" customHeight="1"/>
+    <row r="426" ht="15.75" customHeight="1"/>
+    <row r="427" ht="15.75" customHeight="1"/>
+    <row r="428" ht="15.75" customHeight="1"/>
+    <row r="429" ht="15.75" customHeight="1"/>
+    <row r="430" ht="15.75" customHeight="1"/>
+    <row r="431" ht="15.75" customHeight="1"/>
+    <row r="432" ht="15.75" customHeight="1"/>
+    <row r="433" ht="15.75" customHeight="1"/>
+    <row r="434" ht="15.75" customHeight="1"/>
+    <row r="435" ht="15.75" customHeight="1"/>
+    <row r="436" ht="15.75" customHeight="1"/>
+    <row r="437" ht="15.75" customHeight="1"/>
+    <row r="438" ht="15.75" customHeight="1"/>
+    <row r="439" ht="15.75" customHeight="1"/>
+    <row r="440" ht="15.75" customHeight="1"/>
+    <row r="441" ht="15.75" customHeight="1"/>
+    <row r="442" ht="15.75" customHeight="1"/>
+    <row r="443" ht="15.75" customHeight="1"/>
+    <row r="444" ht="15.75" customHeight="1"/>
+    <row r="445" ht="15.75" customHeight="1"/>
+    <row r="446" ht="15.75" customHeight="1"/>
+    <row r="447" ht="15.75" customHeight="1"/>
+    <row r="448" ht="15.75" customHeight="1"/>
+    <row r="449" ht="15.75" customHeight="1"/>
+    <row r="450" ht="15.75" customHeight="1"/>
+    <row r="451" ht="15.75" customHeight="1"/>
+    <row r="452" ht="15.75" customHeight="1"/>
+    <row r="453" ht="15.75" customHeight="1"/>
+    <row r="454" ht="15.75" customHeight="1"/>
+    <row r="455" ht="15.75" customHeight="1"/>
+    <row r="456" ht="15.75" customHeight="1"/>
+    <row r="457" ht="15.75" customHeight="1"/>
+    <row r="458" ht="15.75" customHeight="1"/>
+    <row r="459" ht="15.75" customHeight="1"/>
+    <row r="460" ht="15.75" customHeight="1"/>
+    <row r="461" ht="15.75" customHeight="1"/>
+    <row r="462" ht="15.75" customHeight="1"/>
+    <row r="463" ht="15.75" customHeight="1"/>
+    <row r="464" ht="15.75" customHeight="1"/>
+    <row r="465" ht="15.75" customHeight="1"/>
+    <row r="466" ht="15.75" customHeight="1"/>
+    <row r="467" ht="15.75" customHeight="1"/>
+    <row r="468" ht="15.75" customHeight="1"/>
+    <row r="469" ht="15.75" customHeight="1"/>
+    <row r="470" ht="15.75" customHeight="1"/>
+    <row r="471" ht="15.75" customHeight="1"/>
+    <row r="472" ht="15.75" customHeight="1"/>
+    <row r="473" ht="15.75" customHeight="1"/>
+    <row r="474" ht="15.75" customHeight="1"/>
+    <row r="475" ht="15.75" customHeight="1"/>
+    <row r="476" ht="15.75" customHeight="1"/>
+    <row r="477" ht="15.75" customHeight="1"/>
+    <row r="478" ht="15.75" customHeight="1"/>
+    <row r="479" ht="15.75" customHeight="1"/>
+    <row r="480" ht="15.75" customHeight="1"/>
+    <row r="481" ht="15.75" customHeight="1"/>
+    <row r="482" ht="15.75" customHeight="1"/>
+    <row r="483" ht="15.75" customHeight="1"/>
+    <row r="484" ht="15.75" customHeight="1"/>
+    <row r="485" ht="15.75" customHeight="1"/>
+    <row r="486" ht="15.75" customHeight="1"/>
+    <row r="487" ht="15.75" customHeight="1"/>
+    <row r="488" ht="15.75" customHeight="1"/>
+    <row r="489" ht="15.75" customHeight="1"/>
+    <row r="490" ht="15.75" customHeight="1"/>
+    <row r="491" ht="15.75" customHeight="1"/>
+    <row r="492" ht="15.75" customHeight="1"/>
+    <row r="493" ht="15.75" customHeight="1"/>
+    <row r="494" ht="15.75" customHeight="1"/>
+    <row r="495" ht="15.75" customHeight="1"/>
+    <row r="496" ht="15.75" customHeight="1"/>
+    <row r="497" ht="15.75" customHeight="1"/>
+    <row r="498" ht="15.75" customHeight="1"/>
+    <row r="499" ht="15.75" customHeight="1"/>
+    <row r="500" ht="15.75" customHeight="1"/>
+    <row r="501" ht="15.75" customHeight="1"/>
+    <row r="502" ht="15.75" customHeight="1"/>
+    <row r="503" ht="15.75" customHeight="1"/>
+    <row r="504" ht="15.75" customHeight="1"/>
+    <row r="505" ht="15.75" customHeight="1"/>
+    <row r="506" ht="15.75" customHeight="1"/>
+    <row r="507" ht="15.75" customHeight="1"/>
+    <row r="508" ht="15.75" customHeight="1"/>
+    <row r="509" ht="15.75" customHeight="1"/>
+    <row r="510" ht="15.75" customHeight="1"/>
+    <row r="511" ht="15.75" customHeight="1"/>
+    <row r="512" ht="15.75" customHeight="1"/>
+    <row r="513" ht="15.75" customHeight="1"/>
+    <row r="514" ht="15.75" customHeight="1"/>
+    <row r="515" ht="15.75" customHeight="1"/>
+    <row r="516" ht="15.75" customHeight="1"/>
+    <row r="517" ht="15.75" customHeight="1"/>
+    <row r="518" ht="15.75" customHeight="1"/>
+    <row r="519" ht="15.75" customHeight="1"/>
+    <row r="520" ht="15.75" customHeight="1"/>
+    <row r="521" ht="15.75" customHeight="1"/>
+    <row r="522" ht="15.75" customHeight="1"/>
+    <row r="523" ht="15.75" customHeight="1"/>
+    <row r="524" ht="15.75" customHeight="1"/>
+    <row r="525" ht="15.75" customHeight="1"/>
+    <row r="526" ht="15.75" customHeight="1"/>
+    <row r="527" ht="15.75" customHeight="1"/>
+    <row r="528" ht="15.75" customHeight="1"/>
+    <row r="529" ht="15.75" customHeight="1"/>
+    <row r="530" ht="15.75" customHeight="1"/>
+    <row r="531" ht="15.75" customHeight="1"/>
+    <row r="532" ht="15.75" customHeight="1"/>
+    <row r="533" ht="15.75" customHeight="1"/>
+    <row r="534" ht="15.75" customHeight="1"/>
+    <row r="535" ht="15.75" customHeight="1"/>
+    <row r="536" ht="15.75" customHeight="1"/>
+    <row r="537" ht="15.75" customHeight="1"/>
+    <row r="538" ht="15.75" customHeight="1"/>
+    <row r="539" ht="15.75" customHeight="1"/>
+    <row r="540" ht="15.75" customHeight="1"/>
+    <row r="541" ht="15.75" customHeight="1"/>
+    <row r="542" ht="15.75" customHeight="1"/>
+    <row r="543" ht="15.75" customHeight="1"/>
+    <row r="544" ht="15.75" customHeight="1"/>
+    <row r="545" ht="15.75" customHeight="1"/>
+    <row r="546" ht="15.75" customHeight="1"/>
+    <row r="547" ht="15.75" customHeight="1"/>
+    <row r="548" ht="15.75" customHeight="1"/>
+    <row r="549" ht="15.75" customHeight="1"/>
+    <row r="550" ht="15.75" customHeight="1"/>
+    <row r="551" ht="15.75" customHeight="1"/>
+    <row r="552" ht="15.75" customHeight="1"/>
+    <row r="553" ht="15.75" customHeight="1"/>
+    <row r="554" ht="15.75" customHeight="1"/>
+    <row r="555" ht="15.75" customHeight="1"/>
+    <row r="556" ht="15.75" customHeight="1"/>
+    <row r="557" ht="15.75" customHeight="1"/>
+    <row r="558" ht="15.75" customHeight="1"/>
+    <row r="559" ht="15.75" customHeight="1"/>
+    <row r="560" ht="15.75" customHeight="1"/>
+    <row r="561" ht="15.75" customHeight="1"/>
+    <row r="562" ht="15.75" customHeight="1"/>
+    <row r="563" ht="15.75" customHeight="1"/>
+    <row r="564" ht="15.75" customHeight="1"/>
+    <row r="565" ht="15.75" customHeight="1"/>
+    <row r="566" ht="15.75" customHeight="1"/>
+    <row r="567" ht="15.75" customHeight="1"/>
+    <row r="568" ht="15.75" customHeight="1"/>
+    <row r="569" ht="15.75" customHeight="1"/>
+    <row r="570" ht="15.75" customHeight="1"/>
+    <row r="571" ht="15.75" customHeight="1"/>
+    <row r="572" ht="15.75" customHeight="1"/>
+    <row r="573" ht="15.75" customHeight="1"/>
+    <row r="574" ht="15.75" customHeight="1"/>
+    <row r="575" ht="15.75" customHeight="1"/>
+    <row r="576" ht="15.75" customHeight="1"/>
+    <row r="577" ht="15.75" customHeight="1"/>
+    <row r="578" ht="15.75" customHeight="1"/>
+    <row r="579" ht="15.75" customHeight="1"/>
+    <row r="580" ht="15.75" customHeight="1"/>
+    <row r="581" ht="15.75" customHeight="1"/>
+    <row r="582" ht="15.75" customHeight="1"/>
+    <row r="583" ht="15.75" customHeight="1"/>
+    <row r="584" ht="15.75" customHeight="1"/>
+    <row r="585" ht="15.75" customHeight="1"/>
+    <row r="586" ht="15.75" customHeight="1"/>
+    <row r="587" ht="15.75" customHeight="1"/>
+    <row r="588" ht="15.75" customHeight="1"/>
+    <row r="589" ht="15.75" customHeight="1"/>
+    <row r="590" ht="15.75" customHeight="1"/>
+    <row r="591" ht="15.75" customHeight="1"/>
+    <row r="592" ht="15.75" customHeight="1"/>
+    <row r="593" ht="15.75" customHeight="1"/>
+    <row r="594" ht="15.75" customHeight="1"/>
+    <row r="595" ht="15.75" customHeight="1"/>
+    <row r="596" ht="15.75" customHeight="1"/>
+    <row r="597" ht="15.75" customHeight="1"/>
+    <row r="598" ht="15.75" customHeight="1"/>
+    <row r="599" ht="15.75" customHeight="1"/>
+    <row r="600" ht="15.75" customHeight="1"/>
+    <row r="601" ht="15.75" customHeight="1"/>
+    <row r="602" ht="15.75" customHeight="1"/>
+    <row r="603" ht="15.75" customHeight="1"/>
+    <row r="604" ht="15.75" customHeight="1"/>
+    <row r="605" ht="15.75" customHeight="1"/>
+    <row r="606" ht="15.75" customHeight="1"/>
+    <row r="607" ht="15.75" customHeight="1"/>
+    <row r="608" ht="15.75" customHeight="1"/>
+    <row r="609" ht="15.75" customHeight="1"/>
+    <row r="610" ht="15.75" customHeight="1"/>
+    <row r="611" ht="15.75" customHeight="1"/>
+    <row r="612" ht="15.75" customHeight="1"/>
+    <row r="613" ht="15.75" customHeight="1"/>
+    <row r="614" ht="15.75" customHeight="1"/>
+    <row r="615" ht="15.75" customHeight="1"/>
+    <row r="616" ht="15.75" customHeight="1"/>
+    <row r="617" ht="15.75" customHeight="1"/>
+    <row r="618" ht="15.75" customHeight="1"/>
+    <row r="619" ht="15.75" customHeight="1"/>
+    <row r="620" ht="15.75" customHeight="1"/>
+    <row r="621" ht="15.75" customHeight="1"/>
+    <row r="622" ht="15.75" customHeight="1"/>
+    <row r="623" ht="15.75" customHeight="1"/>
+    <row r="624" ht="15.75" customHeight="1"/>
+    <row r="625" ht="15.75" customHeight="1"/>
+    <row r="626" ht="15.75" customHeight="1"/>
+    <row r="627" ht="15.75" customHeight="1"/>
+    <row r="628" ht="15.75" customHeight="1"/>
+    <row r="629" ht="15.75" customHeight="1"/>
+    <row r="630" ht="15.75" customHeight="1"/>
+    <row r="631" ht="15.75" customHeight="1"/>
+    <row r="632" ht="15.75" customHeight="1"/>
+    <row r="633" ht="15.75" customHeight="1"/>
+    <row r="634" ht="15.75" customHeight="1"/>
+    <row r="635" ht="15.75" customHeight="1"/>
+    <row r="636" ht="15.75" customHeight="1"/>
+    <row r="637" ht="15.75" customHeight="1"/>
+    <row r="638" ht="15.75" customHeight="1"/>
+    <row r="639" ht="15.75" customHeight="1"/>
+    <row r="640" ht="15.75" customHeight="1"/>
+    <row r="641" ht="15.75" customHeight="1"/>
+    <row r="642" ht="15.75" customHeight="1"/>
+    <row r="643" ht="15.75" customHeight="1"/>
+    <row r="644" ht="15.75" customHeight="1"/>
+    <row r="645" ht="15.75" customHeight="1"/>
+    <row r="646" ht="15.75" customHeight="1"/>
+    <row r="647" ht="15.75" customHeight="1"/>
+    <row r="648" ht="15.75" customHeight="1"/>
+    <row r="649" ht="15.75" customHeight="1"/>
+    <row r="650" ht="15.75" customHeight="1"/>
+    <row r="651" ht="15.75" customHeight="1"/>
+    <row r="652" ht="15.75" customHeight="1"/>
+    <row r="653" ht="15.75" customHeight="1"/>
+    <row r="654" ht="15.75" customHeight="1"/>
+    <row r="655" ht="15.75" customHeight="1"/>
+    <row r="656" ht="15.75" customHeight="1"/>
+    <row r="657" ht="15.75" customHeight="1"/>
+    <row r="658" ht="15.75" customHeight="1"/>
+    <row r="659" ht="15.75" customHeight="1"/>
+    <row r="660" ht="15.75" customHeight="1"/>
+    <row r="661" ht="15.75" customHeight="1"/>
+    <row r="662" ht="15.75" customHeight="1"/>
+    <row r="663" ht="15.75" customHeight="1"/>
+    <row r="664" ht="15.75" customHeight="1"/>
+    <row r="665" ht="15.75" customHeight="1"/>
+    <row r="666" ht="15.75" customHeight="1"/>
+    <row r="667" ht="15.75" customHeight="1"/>
+    <row r="668" ht="15.75" customHeight="1"/>
+    <row r="669" ht="15.75" customHeight="1"/>
+    <row r="670" ht="15.75" customHeight="1"/>
+    <row r="671" ht="15.75" customHeight="1"/>
+    <row r="672" ht="15.75" customHeight="1"/>
+    <row r="673" ht="15.75" customHeight="1"/>
+    <row r="674" ht="15.75" customHeight="1"/>
+    <row r="675" ht="15.75" customHeight="1"/>
+    <row r="676" ht="15.75" customHeight="1"/>
+    <row r="677" ht="15.75" customHeight="1"/>
+    <row r="678" ht="15.75" customHeight="1"/>
+    <row r="679" ht="15.75" customHeight="1"/>
+    <row r="680" ht="15.75" customHeight="1"/>
+    <row r="681" ht="15.75" customHeight="1"/>
+    <row r="682" ht="15.75" customHeight="1"/>
+    <row r="683" ht="15.75" customHeight="1"/>
+    <row r="684" ht="15.75" customHeight="1"/>
+    <row r="685" ht="15.75" customHeight="1"/>
+    <row r="686" ht="15.75" customHeight="1"/>
+    <row r="687" ht="15.75" customHeight="1"/>
+    <row r="688" ht="15.75" customHeight="1"/>
+    <row r="689" ht="15.75" customHeight="1"/>
+    <row r="690" ht="15.75" customHeight="1"/>
+    <row r="691" ht="15.75" customHeight="1"/>
+    <row r="692" ht="15.75" customHeight="1"/>
+    <row r="693" ht="15.75" customHeight="1"/>
+    <row r="694" ht="15.75" customHeight="1"/>
+    <row r="695" ht="15.75" customHeight="1"/>
+    <row r="696" ht="15.75" customHeight="1"/>
+    <row r="697" ht="15.75" customHeight="1"/>
+    <row r="698" ht="15.75" customHeight="1"/>
+    <row r="699" ht="15.75" customHeight="1"/>
+    <row r="700" ht="15.75" customHeight="1"/>
+    <row r="701" ht="15.75" customHeight="1"/>
+    <row r="702" ht="15.75" customHeight="1"/>
+    <row r="703" ht="15.75" customHeight="1"/>
+    <row r="704" ht="15.75" customHeight="1"/>
+    <row r="705" ht="15.75" customHeight="1"/>
+    <row r="706" ht="15.75" customHeight="1"/>
+    <row r="707" ht="15.75" customHeight="1"/>
+    <row r="708" ht="15.75" customHeight="1"/>
+    <row r="709" ht="15.75" customHeight="1"/>
+    <row r="710" ht="15.75" customHeight="1"/>
+    <row r="711" ht="15.75" customHeight="1"/>
+    <row r="712" ht="15.75" customHeight="1"/>
+    <row r="713" ht="15.75" customHeight="1"/>
+    <row r="714" ht="15.75" customHeight="1"/>
+    <row r="715" ht="15.75" customHeight="1"/>
+    <row r="716" ht="15.75" customHeight="1"/>
+    <row r="717" ht="15.75" customHeight="1"/>
+    <row r="718" ht="15.75" customHeight="1"/>
+    <row r="719" ht="15.75" customHeight="1"/>
+    <row r="720" ht="15.75" customHeight="1"/>
+    <row r="721" ht="15.75" customHeight="1"/>
+    <row r="722" ht="15.75" customHeight="1"/>
+    <row r="723" ht="15.75" customHeight="1"/>
+    <row r="724" ht="15.75" customHeight="1"/>
+    <row r="725" ht="15.75" customHeight="1"/>
+    <row r="726" ht="15.75" customHeight="1"/>
+    <row r="727" ht="15.75" customHeight="1"/>
+    <row r="728" ht="15.75" customHeight="1"/>
+    <row r="729" ht="15.75" customHeight="1"/>
+    <row r="730" ht="15.75" customHeight="1"/>
+    <row r="731" ht="15.75" customHeight="1"/>
+    <row r="732" ht="15.75" customHeight="1"/>
+    <row r="733" ht="15.75" customHeight="1"/>
+    <row r="734" ht="15.75" customHeight="1"/>
+    <row r="735" ht="15.75" customHeight="1"/>
+    <row r="736" ht="15.75" customHeight="1"/>
+    <row r="737" ht="15.75" customHeight="1"/>
+    <row r="738" ht="15.75" customHeight="1"/>
+    <row r="739" ht="15.75" customHeight="1"/>
+    <row r="740" ht="15.75" customHeight="1"/>
+    <row r="741" ht="15.75" customHeight="1"/>
+    <row r="742" ht="15.75" customHeight="1"/>
+    <row r="743" ht="15.75" customHeight="1"/>
+    <row r="744" ht="15.75" customHeight="1"/>
+    <row r="745" ht="15.75" customHeight="1"/>
+    <row r="746" ht="15.75" customHeight="1"/>
+    <row r="747" ht="15.75" customHeight="1"/>
+    <row r="748" ht="15.75" customHeight="1"/>
+    <row r="749" ht="15.75" customHeight="1"/>
+    <row r="750" ht="15.75" customHeight="1"/>
+    <row r="751" ht="15.75" customHeight="1"/>
+    <row r="752" ht="15.75" customHeight="1"/>
+    <row r="753" ht="15.75" customHeight="1"/>
+    <row r="754" ht="15.75" customHeight="1"/>
+    <row r="755" ht="15.75" customHeight="1"/>
+    <row r="756" ht="15.75" customHeight="1"/>
+    <row r="757" ht="15.75" customHeight="1"/>
+    <row r="758" ht="15.75" customHeight="1"/>
+    <row r="759" ht="15.75" customHeight="1"/>
+    <row r="760" ht="15.75" customHeight="1"/>
+    <row r="761" ht="15.75" customHeight="1"/>
+    <row r="762" ht="15.75" customHeight="1"/>
+    <row r="763" ht="15.75" customHeight="1"/>
+    <row r="764" ht="15.75" customHeight="1"/>
+    <row r="765" ht="15.75" customHeight="1"/>
+    <row r="766" ht="15.75" customHeight="1"/>
+    <row r="767" ht="15.75" customHeight="1"/>
+    <row r="768" ht="15.75" customHeight="1"/>
+    <row r="769" ht="15.75" customHeight="1"/>
+    <row r="770" ht="15.75" customHeight="1"/>
+    <row r="771" ht="15.75" customHeight="1"/>
+    <row r="772" ht="15.75" customHeight="1"/>
+    <row r="773" ht="15.75" customHeight="1"/>
+    <row r="774" ht="15.75" customHeight="1"/>
+    <row r="775" ht="15.75" customHeight="1"/>
+    <row r="776" ht="15.75" customHeight="1"/>
+    <row r="777" ht="15.75" customHeight="1"/>
+    <row r="778" ht="15.75" customHeight="1"/>
+    <row r="779" ht="15.75" customHeight="1"/>
+    <row r="780" ht="15.75" customHeight="1"/>
+    <row r="781" ht="15.75" customHeight="1"/>
+    <row r="782" ht="15.75" customHeight="1"/>
+    <row r="783" ht="15.75" customHeight="1"/>
+    <row r="784" ht="15.75" customHeight="1"/>
+    <row r="785" ht="15.75" customHeight="1"/>
+    <row r="786" ht="15.75" customHeight="1"/>
+    <row r="787" ht="15.75" customHeight="1"/>
+    <row r="788" ht="15.75" customHeight="1"/>
+    <row r="789" ht="15.75" customHeight="1"/>
+    <row r="790" ht="15.75" customHeight="1"/>
+    <row r="791" ht="15.75" customHeight="1"/>
+    <row r="792" ht="15.75" customHeight="1"/>
+    <row r="793" ht="15.75" customHeight="1"/>
+    <row r="794" ht="15.75" customHeight="1"/>
+    <row r="795" ht="15.75" customHeight="1"/>
+    <row r="796" ht="15.75" customHeight="1"/>
+    <row r="797" ht="15.75" customHeight="1"/>
+    <row r="798" ht="15.75" customHeight="1"/>
+    <row r="799" ht="15.75" customHeight="1"/>
+    <row r="800" ht="15.75" customHeight="1"/>
+    <row r="801" ht="15.75" customHeight="1"/>
+    <row r="802" ht="15.75" customHeight="1"/>
+    <row r="803" ht="15.75" customHeight="1"/>
+    <row r="804" ht="15.75" customHeight="1"/>
+    <row r="805" ht="15.75" customHeight="1"/>
+    <row r="806" ht="15.75" customHeight="1"/>
+    <row r="807" ht="15.75" customHeight="1"/>
+    <row r="808" ht="15.75" customHeight="1"/>
+    <row r="809" ht="15.75" customHeight="1"/>
+    <row r="810" ht="15.75" customHeight="1"/>
+    <row r="811" ht="15.75" customHeight="1"/>
+    <row r="812" ht="15.75" customHeight="1"/>
+    <row r="813" ht="15.75" customHeight="1"/>
+    <row r="814" ht="15.75" customHeight="1"/>
+    <row r="815" ht="15.75" customHeight="1"/>
+    <row r="816" ht="15.75" customHeight="1"/>
+    <row r="817" ht="15.75" customHeight="1"/>
+    <row r="818" ht="15.75" customHeight="1"/>
+    <row r="819" ht="15.75" customHeight="1"/>
+    <row r="820" ht="15.75" customHeight="1"/>
+    <row r="821" ht="15.75" customHeight="1"/>
+    <row r="822" ht="15.75" customHeight="1"/>
+    <row r="823" ht="15.75" customHeight="1"/>
+    <row r="824" ht="15.75" customHeight="1"/>
+    <row r="825" ht="15.75" customHeight="1"/>
+    <row r="826" ht="15.75" customHeight="1"/>
+    <row r="827" ht="15.75" customHeight="1"/>
+    <row r="828" ht="15.75" customHeight="1"/>
+    <row r="829" ht="15.75" customHeight="1"/>
+    <row r="830" ht="15.75" customHeight="1"/>
+    <row r="831" ht="15.75" customHeight="1"/>
+    <row r="832" ht="15.75" customHeight="1"/>
+    <row r="833" ht="15.75" customHeight="1"/>
+    <row r="834" ht="15.75" customHeight="1"/>
+    <row r="835" ht="15.75" customHeight="1"/>
+    <row r="836" ht="15.75" customHeight="1"/>
+    <row r="837" ht="15.75" customHeight="1"/>
+    <row r="838" ht="15.75" customHeight="1"/>
+    <row r="839" ht="15.75" customHeight="1"/>
+    <row r="840" ht="15.75" customHeight="1"/>
+    <row r="841" ht="15.75" customHeight="1"/>
+    <row r="842" ht="15.75" customHeight="1"/>
+    <row r="843" ht="15.75" customHeight="1"/>
+    <row r="844" ht="15.75" customHeight="1"/>
+    <row r="845" ht="15.75" customHeight="1"/>
+    <row r="846" ht="15.75" customHeight="1"/>
+    <row r="847" ht="15.75" customHeight="1"/>
+    <row r="848" ht="15.75" customHeight="1"/>
+    <row r="849" ht="15.75" customHeight="1"/>
+    <row r="850" ht="15.75" customHeight="1"/>
+    <row r="851" ht="15.75" customHeight="1"/>
+    <row r="852" ht="15.75" customHeight="1"/>
+    <row r="853" ht="15.75" customHeight="1"/>
+    <row r="854" ht="15.75" customHeight="1"/>
+    <row r="855" ht="15.75" customHeight="1"/>
+    <row r="856" ht="15.75" customHeight="1"/>
+    <row r="857" ht="15.75" customHeight="1"/>
+    <row r="858" ht="15.75" customHeight="1"/>
+    <row r="859" ht="15.75" customHeight="1"/>
+    <row r="860" ht="15.75" customHeight="1"/>
+    <row r="861" ht="15.75" customHeight="1"/>
+    <row r="862" ht="15.75" customHeight="1"/>
+    <row r="863" ht="15.75" customHeight="1"/>
+    <row r="864" ht="15.75" customHeight="1"/>
+    <row r="865" ht="15.75" customHeight="1"/>
+    <row r="866" ht="15.75" customHeight="1"/>
+    <row r="867" ht="15.75" customHeight="1"/>
+    <row r="868" ht="15.75" customHeight="1"/>
+    <row r="869" ht="15.75" customHeight="1"/>
+    <row r="870" ht="15.75" customHeight="1"/>
+    <row r="871" ht="15.75" customHeight="1"/>
+    <row r="872" ht="15.75" customHeight="1"/>
+    <row r="873" ht="15.75" customHeight="1"/>
+    <row r="874" ht="15.75" customHeight="1"/>
+    <row r="875" ht="15.75" customHeight="1"/>
+    <row r="876" ht="15.75" customHeight="1"/>
+    <row r="877" ht="15.75" customHeight="1"/>
+    <row r="878" ht="15.75" customHeight="1"/>
+    <row r="879" ht="15.75" customHeight="1"/>
+    <row r="880" ht="15.75" customHeight="1"/>
+    <row r="881" ht="15.75" customHeight="1"/>
+    <row r="882" ht="15.75" customHeight="1"/>
+    <row r="883" ht="15.75" customHeight="1"/>
+    <row r="884" ht="15.75" customHeight="1"/>
+    <row r="885" ht="15.75" customHeight="1"/>
+    <row r="886" ht="15.75" customHeight="1"/>
+    <row r="887" ht="15.75" customHeight="1"/>
+    <row r="888" ht="15.75" customHeight="1"/>
+    <row r="889" ht="15.75" customHeight="1"/>
+    <row r="890" ht="15.75" customHeight="1"/>
+    <row r="891" ht="15.75" customHeight="1"/>
+    <row r="892" ht="15.75" customHeight="1"/>
+    <row r="893" ht="15.75" customHeight="1"/>
+    <row r="894" ht="15.75" customHeight="1"/>
+    <row r="895" ht="15.75" customHeight="1"/>
+    <row r="896" ht="15.75" customHeight="1"/>
+    <row r="897" ht="15.75" customHeight="1"/>
+    <row r="898" ht="15.75" customHeight="1"/>
+    <row r="899" ht="15.75" customHeight="1"/>
+    <row r="900" ht="15.75" customHeight="1"/>
+    <row r="901" ht="15.75" customHeight="1"/>
+    <row r="902" ht="15.75" customHeight="1"/>
+    <row r="903" ht="15.75" customHeight="1"/>
+    <row r="904" ht="15.75" customHeight="1"/>
+    <row r="905" ht="15.75" customHeight="1"/>
+    <row r="906" ht="15.75" customHeight="1"/>
+    <row r="907" ht="15.75" customHeight="1"/>
+    <row r="908" ht="15.75" customHeight="1"/>
+    <row r="909" ht="15.75" customHeight="1"/>
+    <row r="910" ht="15.75" customHeight="1"/>
+    <row r="911" ht="15.75" customHeight="1"/>
+    <row r="912" ht="15.75" customHeight="1"/>
+    <row r="913" ht="15.75" customHeight="1"/>
+    <row r="914" ht="15.75" customHeight="1"/>
+    <row r="915" ht="15.75" customHeight="1"/>
+    <row r="916" ht="15.75" customHeight="1"/>
+    <row r="917" ht="15.75" customHeight="1"/>
+    <row r="918" ht="15.75" customHeight="1"/>
+    <row r="919" ht="15.75" customHeight="1"/>
+    <row r="920" ht="15.75" customHeight="1"/>
+    <row r="921" ht="15.75" customHeight="1"/>
+    <row r="922" ht="15.75" customHeight="1"/>
+    <row r="923" ht="15.75" customHeight="1"/>
+    <row r="924" ht="15.75" customHeight="1"/>
+    <row r="925" ht="15.75" customHeight="1"/>
+    <row r="926" ht="15.75" customHeight="1"/>
+    <row r="927" ht="15.75" customHeight="1"/>
+    <row r="928" ht="15.75" customHeight="1"/>
+    <row r="929" ht="15.75" customHeight="1"/>
+    <row r="930" ht="15.75" customHeight="1"/>
+    <row r="931" ht="15.75" customHeight="1"/>
+    <row r="932" ht="15.75" customHeight="1"/>
+    <row r="933" ht="15.75" customHeight="1"/>
+    <row r="934" ht="15.75" customHeight="1"/>
+    <row r="935" ht="15.75" customHeight="1"/>
+    <row r="936" ht="15.75" customHeight="1"/>
+    <row r="937" ht="15.75" customHeight="1"/>
+    <row r="938" ht="15.75" customHeight="1"/>
+    <row r="939" ht="15.75" customHeight="1"/>
+    <row r="940" ht="15.75" customHeight="1"/>
+    <row r="941" ht="15.75" customHeight="1"/>
+    <row r="942" ht="15.75" customHeight="1"/>
+    <row r="943" ht="15.75" customHeight="1"/>
+    <row r="944" ht="15.75" customHeight="1"/>
+    <row r="945" ht="15.75" customHeight="1"/>
+    <row r="946" ht="15.75" customHeight="1"/>
+    <row r="947" ht="15.75" customHeight="1"/>
+    <row r="948" ht="15.75" customHeight="1"/>
+    <row r="949" ht="15.75" customHeight="1"/>
+    <row r="950" ht="15.75" customHeight="1"/>
+    <row r="951" ht="15.75" customHeight="1"/>
+    <row r="952" ht="15.75" customHeight="1"/>
+    <row r="953" ht="15.75" customHeight="1"/>
+    <row r="954" ht="15.75" customHeight="1"/>
+    <row r="955" ht="15.75" customHeight="1"/>
+    <row r="956" ht="15.75" customHeight="1"/>
+    <row r="957" ht="15.75" customHeight="1"/>
+    <row r="958" ht="15.75" customHeight="1"/>
+    <row r="959" ht="15.75" customHeight="1"/>
+    <row r="960" ht="15.75" customHeight="1"/>
+    <row r="961" ht="15.75" customHeight="1"/>
+    <row r="962" ht="15.75" customHeight="1"/>
+    <row r="963" ht="15.75" customHeight="1"/>
+    <row r="964" ht="15.75" customHeight="1"/>
+    <row r="965" ht="15.75" customHeight="1"/>
+    <row r="966" ht="15.75" customHeight="1"/>
+    <row r="967" ht="15.75" customHeight="1"/>
+    <row r="968" ht="15.75" customHeight="1"/>
+    <row r="969" ht="15.75" customHeight="1"/>
+    <row r="970" ht="15.75" customHeight="1"/>
+    <row r="971" ht="15.75" customHeight="1"/>
+    <row r="972" ht="15.75" customHeight="1"/>
+    <row r="973" ht="15.75" customHeight="1"/>
+    <row r="974" ht="15.75" customHeight="1"/>
+    <row r="975" ht="15.75" customHeight="1"/>
+    <row r="976" ht="15.75" customHeight="1"/>
+    <row r="977" ht="15.75" customHeight="1"/>
+    <row r="978" ht="15.75" customHeight="1"/>
+    <row r="979" ht="15.75" customHeight="1"/>
+    <row r="980" ht="15.75" customHeight="1"/>
+    <row r="981" ht="15.75" customHeight="1"/>
+    <row r="982" ht="15.75" customHeight="1"/>
+    <row r="983" ht="15.75" customHeight="1"/>
+    <row r="984" ht="15.75" customHeight="1"/>
+    <row r="985" ht="15.75" customHeight="1"/>
+    <row r="986" ht="15.75" customHeight="1"/>
+    <row r="987" ht="15.75" customHeight="1"/>
+    <row r="988" ht="15.75" customHeight="1"/>
+    <row r="989" ht="15.75" customHeight="1"/>
+    <row r="990" ht="15.75" customHeight="1"/>
+    <row r="991" ht="15.75" customHeight="1"/>
+    <row r="992" ht="15.75" customHeight="1"/>
+    <row r="993" ht="15.75" customHeight="1"/>
+    <row r="994" ht="15.75" customHeight="1"/>
+    <row r="995" ht="15.75" customHeight="1"/>
+    <row r="996" ht="15.75" customHeight="1"/>
+    <row r="997" ht="15.75" customHeight="1"/>
+    <row r="998" ht="15.75" customHeight="1"/>
+    <row r="999" ht="15.75" customHeight="1"/>
+    <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <printOptions/>
+  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup orientation="landscape"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>